<commit_message>
new equations for prob
</commit_message>
<xml_diff>
--- a/results/probability_data_2.xlsx
+++ b/results/probability_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisWiseLocal\GitHub\ZEIT3191-ML-Quantum-Computing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73ADEDD-373A-4822-8560-20A5CD03B135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48CAF20-AAB9-4400-AD4E-951FD6E1A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P93" sqref="P93"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,7 +2721,7 @@
         <v>4.0212385965949355</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" ref="H67:H103" si="18">ABS(B67-E67)</f>
+        <f t="shared" ref="H67:H102" si="18">ABS(B67-E67)</f>
         <v>4.2561994874344783E-2</v>
       </c>
       <c r="J67" s="3">

</xml_diff>

<commit_message>
implemented test code and minimised main code
</commit_message>
<xml_diff>
--- a/results/probability_data_2.xlsx
+++ b/results/probability_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisWiseLocal\GitHub\ZEIT3191-ML-Quantum-Computing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48CAF20-AAB9-4400-AD4E-951FD6E1A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FFC34C-D3A5-4AC4-A43B-B7AAC0CC17B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>Ideal probabilities</t>
   </si>
@@ -57,6 +57,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,13 +194,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,6 +216,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,29 +546,33 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="10" max="11" width="19.7109375" customWidth="1"/>
+    <col min="13" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="9"/>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="J1" s="11" t="s">
+      <c r="H1" s="9"/>
+      <c r="J1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K1" s="9"/>
+      <c r="M1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -587,8 +597,14 @@
       <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f t="shared" ref="A3:A34" si="0">(ROW(A3)-ROW($A$3))*PI()/50</f>
         <v>0</v>
@@ -620,8 +636,16 @@
         <f t="shared" ref="K3:K34" si="6">ABS(COS(J3))^2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M66" si="7">(ROW(M3)-ROW($A$3))*PI()/50</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="13">
+        <f>IF(AND(ISEVEN(ROUNDDOWN(E3*10000,1)),ROUNDDOWN(E3*10000,1)&gt;=E3*10000),ROUNDDOWN(E3,4),ROUND(E3,4))</f>
+        <v>0.98780000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" si="0"/>
         <v>6.2831853071795868E-2</v>
@@ -653,8 +677,16 @@
         <f t="shared" si="6"/>
         <v>0.99605735065723888</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="3">
+        <f t="shared" si="7"/>
+        <v>6.2831853071795868E-2</v>
+      </c>
+      <c r="N4" s="13">
+        <f t="shared" ref="N4:N67" si="8">IF(AND(ISEVEN(ROUNDDOWN(E4*10000,1)),ROUNDDOWN(E4*10000,1)&gt;=E4*10000),ROUNDDOWN(E4,4),ROUND(E4,4))</f>
+        <v>0.98740000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>0.12566370614359174</v>
@@ -686,8 +718,16 @@
         <f t="shared" si="6"/>
         <v>0.98429158056431565</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="3">
+        <f t="shared" si="7"/>
+        <v>0.12566370614359174</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" si="8"/>
+        <v>0.98660000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>0.18849555921538758</v>
@@ -719,8 +759,16 @@
         <f t="shared" si="6"/>
         <v>0.96488824294412578</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="3">
+        <f t="shared" si="7"/>
+        <v>0.18849555921538758</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="8"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>0.25132741228718347</v>
@@ -752,8 +800,16 @@
         <f t="shared" si="6"/>
         <v>0.93815334002193174</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.25132741228718347</v>
+      </c>
+      <c r="N7" s="13">
+        <f t="shared" si="8"/>
+        <v>0.97419999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>0.31415926535897931</v>
@@ -785,8 +841,16 @@
         <f t="shared" si="6"/>
         <v>0.90450849718747361</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.31415926535897931</v>
+      </c>
+      <c r="N8" s="13">
+        <f t="shared" si="8"/>
+        <v>0.96609999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>0.37699111843077515</v>
@@ -818,8 +882,16 @@
         <f t="shared" si="6"/>
         <v>0.86448431371070589</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.37699111843077515</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" si="8"/>
+        <v>0.95720000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>0.43982297150257105</v>
@@ -851,8 +923,16 @@
         <f t="shared" si="6"/>
         <v>0.81871199487434498</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="3">
+        <f t="shared" si="7"/>
+        <v>0.43982297150257105</v>
+      </c>
+      <c r="N10" s="13">
+        <f t="shared" si="8"/>
+        <v>0.94489999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>0.50265482457436694</v>
@@ -884,8 +964,16 @@
         <f t="shared" si="6"/>
         <v>0.76791339748949827</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="3">
+        <f t="shared" si="7"/>
+        <v>0.50265482457436694</v>
+      </c>
+      <c r="N11" s="13">
+        <f t="shared" si="8"/>
+        <v>0.93420000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>0.56548667764616278</v>
@@ -917,8 +1005,16 @@
         <f t="shared" si="6"/>
         <v>0.71288964578253633</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="3">
+        <f t="shared" si="7"/>
+        <v>0.56548667764616278</v>
+      </c>
+      <c r="N12" s="13">
+        <f t="shared" si="8"/>
+        <v>0.91810000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>0.62831853071795862</v>
@@ -950,8 +1046,16 @@
         <f t="shared" si="6"/>
         <v>0.65450849718747373</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="3">
+        <f t="shared" si="7"/>
+        <v>0.62831853071795862</v>
+      </c>
+      <c r="N13" s="13">
+        <f t="shared" si="8"/>
+        <v>0.90010000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>0.69115038378975446</v>
@@ -983,8 +1087,16 @@
         <f t="shared" si="6"/>
         <v>0.5936906572928623</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" s="3">
+        <f t="shared" si="7"/>
+        <v>0.69115038378975446</v>
+      </c>
+      <c r="N14" s="13">
+        <f t="shared" si="8"/>
+        <v>0.88160000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>0.7539822368615503</v>
@@ -1016,8 +1128,16 @@
         <f t="shared" si="6"/>
         <v>0.53139525976465674</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15" s="3">
+        <f t="shared" si="7"/>
+        <v>0.7539822368615503</v>
+      </c>
+      <c r="N15" s="13">
+        <f t="shared" si="8"/>
+        <v>0.86760000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>0.81681408993334625</v>
@@ -1049,8 +1169,16 @@
         <f t="shared" si="6"/>
         <v>0.46860474023534321</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="3">
+        <f t="shared" si="7"/>
+        <v>0.81681408993334625</v>
+      </c>
+      <c r="N16" s="13">
+        <f t="shared" si="8"/>
+        <v>0.83940000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>0.87964594300514209</v>
@@ -1082,8 +1210,16 @@
         <f t="shared" si="6"/>
         <v>0.40630934270713776</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17" s="3">
+        <f t="shared" si="7"/>
+        <v>0.87964594300514209</v>
+      </c>
+      <c r="N17" s="13">
+        <f t="shared" si="8"/>
+        <v>0.8226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>0.94247779607693782</v>
@@ -1115,8 +1251,16 @@
         <f t="shared" si="6"/>
         <v>0.34549150281252644</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" s="3">
+        <f t="shared" si="7"/>
+        <v>0.94247779607693782</v>
+      </c>
+      <c r="N18" s="13">
+        <f t="shared" si="8"/>
+        <v>0.79820000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>1.0053096491487339</v>
@@ -1148,8 +1292,16 @@
         <f t="shared" si="6"/>
         <v>0.28711035421746361</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="3">
+        <f t="shared" si="7"/>
+        <v>1.0053096491487339</v>
+      </c>
+      <c r="N19" s="13">
+        <f t="shared" si="8"/>
+        <v>0.7762</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>1.0681415022205298</v>
@@ -1181,8 +1333,16 @@
         <f t="shared" si="6"/>
         <v>0.23208660251050159</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="3">
+        <f t="shared" si="7"/>
+        <v>1.0681415022205298</v>
+      </c>
+      <c r="N20" s="13">
+        <f t="shared" si="8"/>
+        <v>0.74870000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>1.1309733552923256</v>
@@ -1214,8 +1374,16 @@
         <f t="shared" si="6"/>
         <v>0.18128800512565516</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="3">
+        <f t="shared" si="7"/>
+        <v>1.1309733552923256</v>
+      </c>
+      <c r="N21" s="13">
+        <f t="shared" si="8"/>
+        <v>0.71850000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>1.1938052083641213</v>
@@ -1247,8 +1415,16 @@
         <f t="shared" si="6"/>
         <v>0.13551568628929433</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="3">
+        <f t="shared" si="7"/>
+        <v>1.1938052083641213</v>
+      </c>
+      <c r="N22" s="13">
+        <f t="shared" si="8"/>
+        <v>0.69310000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>1.2566370614359172</v>
@@ -1280,8 +1456,16 @@
         <f t="shared" si="6"/>
         <v>9.5491502812526302E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="3">
+        <f t="shared" si="7"/>
+        <v>1.2566370614359172</v>
+      </c>
+      <c r="N23" s="13">
+        <f t="shared" si="8"/>
+        <v>0.6704</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>1.3194689145077132</v>
@@ -1313,8 +1497,16 @@
         <f t="shared" si="6"/>
         <v>6.184665997806818E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" s="3">
+        <f t="shared" si="7"/>
+        <v>1.3194689145077132</v>
+      </c>
+      <c r="N24" s="13">
+        <f t="shared" si="8"/>
+        <v>0.63980000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>1.3823007675795089</v>
@@ -1346,8 +1538,16 @@
         <f t="shared" si="6"/>
         <v>3.511175705587434E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25" s="3">
+        <f t="shared" si="7"/>
+        <v>1.3823007675795089</v>
+      </c>
+      <c r="N25" s="13">
+        <f t="shared" si="8"/>
+        <v>0.61990000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>1.4451326206513047</v>
@@ -1379,8 +1579,16 @@
         <f t="shared" si="6"/>
         <v>1.57084194356845E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="3">
+        <f t="shared" si="7"/>
+        <v>1.4451326206513047</v>
+      </c>
+      <c r="N26" s="13">
+        <f t="shared" si="8"/>
+        <v>0.58179999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>1.5079644737231006</v>
@@ -1412,8 +1620,16 @@
         <f t="shared" si="6"/>
         <v>3.9426493427611037E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27" s="3">
+        <f t="shared" si="7"/>
+        <v>1.5079644737231006</v>
+      </c>
+      <c r="N27" s="13">
+        <f t="shared" si="8"/>
+        <v>0.56279999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>1.5707963267948966</v>
@@ -1445,8 +1661,16 @@
         <f t="shared" si="6"/>
         <v>3.7524718414124473E-33</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28" s="3">
+        <f t="shared" si="7"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="N28" s="13">
+        <f t="shared" si="8"/>
+        <v>0.52139999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>1.6336281798666925</v>
@@ -1478,8 +1702,16 @@
         <f t="shared" si="6"/>
         <v>3.9426493427610881E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29" s="3">
+        <f t="shared" si="7"/>
+        <v>1.6336281798666925</v>
+      </c>
+      <c r="N29" s="13">
+        <f t="shared" si="8"/>
+        <v>0.4924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>1.6964600329384882</v>
@@ -1511,8 +1743,16 @@
         <f t="shared" si="6"/>
         <v>1.5708419435684417E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30" s="3">
+        <f t="shared" si="7"/>
+        <v>1.6964600329384882</v>
+      </c>
+      <c r="N30" s="13">
+        <f t="shared" si="8"/>
+        <v>0.46920000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>1.7592918860102842</v>
@@ -1544,8 +1784,16 @@
         <f t="shared" si="6"/>
         <v>3.5111757055874285E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31" s="3">
+        <f t="shared" si="7"/>
+        <v>1.7592918860102842</v>
+      </c>
+      <c r="N31" s="13">
+        <f t="shared" si="8"/>
+        <v>0.4415</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>1.8221237390820801</v>
@@ -1577,8 +1825,16 @@
         <f t="shared" si="6"/>
         <v>6.1846659978068236E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M32" s="3">
+        <f t="shared" si="7"/>
+        <v>1.8221237390820801</v>
+      </c>
+      <c r="N32" s="13">
+        <f t="shared" si="8"/>
+        <v>0.40820000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>1.8849555921538756</v>
@@ -1610,8 +1866,16 @@
         <f t="shared" si="6"/>
         <v>9.5491502812526094E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33" s="3">
+        <f t="shared" si="7"/>
+        <v>1.8849555921538756</v>
+      </c>
+      <c r="N33" s="13">
+        <f t="shared" si="8"/>
+        <v>0.38479999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>1.9477874452256716</v>
@@ -1643,619 +1907,771 @@
         <f t="shared" si="6"/>
         <v>0.13551568628929408</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M34" s="3">
+        <f t="shared" si="7"/>
+        <v>1.9477874452256716</v>
+      </c>
+      <c r="N34" s="13">
+        <f t="shared" si="8"/>
+        <v>0.3518</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <f t="shared" ref="A35:A66" si="7">(ROW(A35)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="A35:A66" si="9">(ROW(A35)-ROW($A$3))*PI()/50</f>
         <v>2.0106192982974678</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ref="B35:B66" si="8">ABS(COS(A35/2))^2</f>
+        <f t="shared" ref="B35:B66" si="10">ABS(COS(A35/2))^2</f>
         <v>0.28711035421746361</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" ref="D35:D66" si="9">(ROW(D35)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="D35:D66" si="11">(ROW(D35)-ROW($A$3))*PI()/50</f>
         <v>2.0106192982974678</v>
       </c>
       <c r="E35" s="1">
         <v>0.3266</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" ref="G35:G66" si="10">(ROW(G35)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="G35:G66" si="12">(ROW(G35)-ROW($A$3))*PI()/50</f>
         <v>2.0106192982974678</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" ref="H35:H66" si="11">ABS(B35-E35)</f>
+        <f t="shared" ref="H35:H66" si="13">ABS(B35-E35)</f>
         <v>3.9489645782536387E-2</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" ref="J35:J66" si="12">(ROW(J35)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="J35:J66" si="14">(ROW(J35)-ROW($A$3))*PI()/50</f>
         <v>2.0106192982974678</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" ref="K35:K66" si="13">ABS(COS(J35))^2</f>
+        <f t="shared" ref="K35:K66" si="15">ABS(COS(J35))^2</f>
         <v>0.18128800512565521</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M35" s="3">
+        <f t="shared" si="7"/>
+        <v>2.0106192982974678</v>
+      </c>
+      <c r="N35" s="13">
+        <f t="shared" si="8"/>
+        <v>0.3266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <f t="shared" si="7"/>
-        <v>2.0734511513692637</v>
-      </c>
-      <c r="B36" s="1">
-        <f t="shared" si="8"/>
-        <v>0.25912316294914228</v>
-      </c>
-      <c r="D36" s="3">
         <f t="shared" si="9"/>
         <v>2.0734511513692637</v>
       </c>
+      <c r="B36" s="1">
+        <f t="shared" si="10"/>
+        <v>0.25912316294914228</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="11"/>
+        <v>2.0734511513692637</v>
+      </c>
       <c r="E36" s="1">
         <v>0.30304999999999999</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="10"/>
-        <v>2.0734511513692637</v>
-      </c>
-      <c r="H36" s="1">
-        <f t="shared" si="11"/>
-        <v>4.3926837050857703E-2</v>
-      </c>
-      <c r="J36" s="3">
         <f t="shared" si="12"/>
         <v>2.0734511513692637</v>
       </c>
+      <c r="H36" s="1">
+        <f t="shared" si="13"/>
+        <v>4.3926837050857703E-2</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="14"/>
+        <v>2.0734511513692637</v>
+      </c>
       <c r="K36" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.23208660251050184</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M36" s="3">
+        <f t="shared" si="7"/>
+        <v>2.0734511513692637</v>
+      </c>
+      <c r="N36" s="13">
+        <f t="shared" si="8"/>
+        <v>0.30299999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <f t="shared" si="7"/>
-        <v>2.1362830044410597</v>
-      </c>
-      <c r="B37" s="1">
-        <f t="shared" si="8"/>
-        <v>0.23208660251050159</v>
-      </c>
-      <c r="D37" s="3">
         <f t="shared" si="9"/>
         <v>2.1362830044410597</v>
       </c>
+      <c r="B37" s="1">
+        <f t="shared" si="10"/>
+        <v>0.23208660251050159</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="11"/>
+        <v>2.1362830044410597</v>
+      </c>
       <c r="E37" s="1">
         <v>0.27374999999999999</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="10"/>
-        <v>2.1362830044410597</v>
-      </c>
-      <c r="H37" s="1">
-        <f t="shared" si="11"/>
-        <v>4.1663397489498405E-2</v>
-      </c>
-      <c r="J37" s="3">
         <f t="shared" si="12"/>
         <v>2.1362830044410597</v>
       </c>
+      <c r="H37" s="1">
+        <f t="shared" si="13"/>
+        <v>4.1663397489498405E-2</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="14"/>
+        <v>2.1362830044410597</v>
+      </c>
       <c r="K37" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.28711035421746395</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M37" s="3">
+        <f t="shared" si="7"/>
+        <v>2.1362830044410597</v>
+      </c>
+      <c r="N37" s="13">
+        <f t="shared" si="8"/>
+        <v>0.27379999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <f t="shared" si="7"/>
-        <v>2.1991148575128552</v>
-      </c>
-      <c r="B38" s="1">
-        <f t="shared" si="8"/>
-        <v>0.20610737385376346</v>
-      </c>
-      <c r="D38" s="3">
         <f t="shared" si="9"/>
         <v>2.1991148575128552</v>
       </c>
+      <c r="B38" s="1">
+        <f t="shared" si="10"/>
+        <v>0.20610737385376346</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="11"/>
+        <v>2.1991148575128552</v>
+      </c>
       <c r="E38" s="1">
         <v>0.25595000000000001</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="10"/>
-        <v>2.1991148575128552</v>
-      </c>
-      <c r="H38" s="1">
-        <f t="shared" si="11"/>
-        <v>4.9842626146236552E-2</v>
-      </c>
-      <c r="J38" s="3">
         <f t="shared" si="12"/>
         <v>2.1991148575128552</v>
       </c>
+      <c r="H38" s="1">
+        <f t="shared" si="13"/>
+        <v>4.9842626146236552E-2</v>
+      </c>
+      <c r="J38" s="3">
+        <f t="shared" si="14"/>
+        <v>2.1991148575128552</v>
+      </c>
       <c r="K38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.34549150281252616</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M38" s="3">
+        <f t="shared" si="7"/>
+        <v>2.1991148575128552</v>
+      </c>
+      <c r="N38" s="13">
+        <f t="shared" si="8"/>
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <f t="shared" si="7"/>
-        <v>2.2619467105846511</v>
-      </c>
-      <c r="B39" s="1">
-        <f t="shared" si="8"/>
-        <v>0.18128800512565516</v>
-      </c>
-      <c r="D39" s="3">
         <f t="shared" si="9"/>
         <v>2.2619467105846511</v>
       </c>
+      <c r="B39" s="1">
+        <f t="shared" si="10"/>
+        <v>0.18128800512565516</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="11"/>
+        <v>2.2619467105846511</v>
+      </c>
       <c r="E39" s="1">
         <v>0.23100000000000001</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" si="10"/>
-        <v>2.2619467105846511</v>
-      </c>
-      <c r="H39" s="1">
-        <f t="shared" si="11"/>
-        <v>4.9711994874344856E-2</v>
-      </c>
-      <c r="J39" s="3">
         <f t="shared" si="12"/>
         <v>2.2619467105846511</v>
       </c>
+      <c r="H39" s="1">
+        <f t="shared" si="13"/>
+        <v>4.9711994874344856E-2</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="14"/>
+        <v>2.2619467105846511</v>
+      </c>
       <c r="K39" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.40630934270713776</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M39" s="3">
+        <f t="shared" si="7"/>
+        <v>2.2619467105846511</v>
+      </c>
+      <c r="N39" s="13">
+        <f t="shared" si="8"/>
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <f t="shared" si="7"/>
-        <v>2.3247785636564471</v>
-      </c>
-      <c r="B40" s="1">
-        <f t="shared" si="8"/>
-        <v>0.15772644703565564</v>
-      </c>
-      <c r="D40" s="3">
         <f t="shared" si="9"/>
         <v>2.3247785636564471</v>
       </c>
+      <c r="B40" s="1">
+        <f t="shared" si="10"/>
+        <v>0.15772644703565564</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="11"/>
+        <v>2.3247785636564471</v>
+      </c>
       <c r="E40" s="1">
         <v>0.20910000000000001</v>
       </c>
       <c r="G40" s="3">
-        <f t="shared" si="10"/>
-        <v>2.3247785636564471</v>
-      </c>
-      <c r="H40" s="1">
-        <f t="shared" si="11"/>
-        <v>5.1373552964344371E-2</v>
-      </c>
-      <c r="J40" s="3">
         <f t="shared" si="12"/>
         <v>2.3247785636564471</v>
       </c>
+      <c r="H40" s="1">
+        <f t="shared" si="13"/>
+        <v>5.1373552964344371E-2</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="14"/>
+        <v>2.3247785636564471</v>
+      </c>
       <c r="K40" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.46860474023534338</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M40" s="3">
+        <f t="shared" si="7"/>
+        <v>2.3247785636564471</v>
+      </c>
+      <c r="N40" s="13">
+        <f t="shared" si="8"/>
+        <v>0.20910000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <f t="shared" si="7"/>
-        <v>2.3876104167282426</v>
-      </c>
-      <c r="B41" s="1">
-        <f t="shared" si="8"/>
-        <v>0.13551568628929433</v>
-      </c>
-      <c r="D41" s="3">
         <f t="shared" si="9"/>
         <v>2.3876104167282426</v>
       </c>
+      <c r="B41" s="1">
+        <f t="shared" si="10"/>
+        <v>0.13551568628929433</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="11"/>
+        <v>2.3876104167282426</v>
+      </c>
       <c r="E41" s="1">
         <v>0.18675</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" si="10"/>
-        <v>2.3876104167282426</v>
-      </c>
-      <c r="H41" s="1">
-        <f t="shared" si="11"/>
-        <v>5.1234313710705665E-2</v>
-      </c>
-      <c r="J41" s="3">
         <f t="shared" si="12"/>
         <v>2.3876104167282426</v>
       </c>
+      <c r="H41" s="1">
+        <f t="shared" si="13"/>
+        <v>5.1234313710705665E-2</v>
+      </c>
+      <c r="J41" s="3">
+        <f t="shared" si="14"/>
+        <v>2.3876104167282426</v>
+      </c>
       <c r="K41" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.5313952597646564</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M41" s="3">
+        <f t="shared" si="7"/>
+        <v>2.3876104167282426</v>
+      </c>
+      <c r="N41" s="13">
+        <f t="shared" si="8"/>
+        <v>0.18679999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <f t="shared" si="7"/>
-        <v>2.4504422698000385</v>
-      </c>
-      <c r="B42" s="1">
-        <f t="shared" si="8"/>
-        <v>0.11474337861210546</v>
-      </c>
-      <c r="D42" s="3">
         <f t="shared" si="9"/>
         <v>2.4504422698000385</v>
       </c>
+      <c r="B42" s="1">
+        <f t="shared" si="10"/>
+        <v>0.11474337861210546</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="11"/>
+        <v>2.4504422698000385</v>
+      </c>
       <c r="E42" s="1">
         <v>0.16650000000000001</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="10"/>
-        <v>2.4504422698000385</v>
-      </c>
-      <c r="H42" s="1">
-        <f t="shared" si="11"/>
-        <v>5.1756621387894552E-2</v>
-      </c>
-      <c r="J42" s="3">
         <f t="shared" si="12"/>
         <v>2.4504422698000385</v>
       </c>
+      <c r="H42" s="1">
+        <f t="shared" si="13"/>
+        <v>5.1756621387894552E-2</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="14"/>
+        <v>2.4504422698000385</v>
+      </c>
       <c r="K42" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.59369065729286219</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M42" s="3">
+        <f t="shared" si="7"/>
+        <v>2.4504422698000385</v>
+      </c>
+      <c r="N42" s="13">
+        <f t="shared" si="8"/>
+        <v>0.16650000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <f t="shared" si="7"/>
-        <v>2.5132741228718345</v>
-      </c>
-      <c r="B43" s="1">
-        <f t="shared" si="8"/>
-        <v>9.5491502812526302E-2</v>
-      </c>
-      <c r="D43" s="3">
         <f t="shared" si="9"/>
         <v>2.5132741228718345</v>
       </c>
+      <c r="B43" s="1">
+        <f t="shared" si="10"/>
+        <v>9.5491502812526302E-2</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="11"/>
+        <v>2.5132741228718345</v>
+      </c>
       <c r="E43" s="1">
         <v>0.15190000000000001</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" si="10"/>
-        <v>2.5132741228718345</v>
-      </c>
-      <c r="H43" s="1">
-        <f t="shared" si="11"/>
-        <v>5.6408497187473705E-2</v>
-      </c>
-      <c r="J43" s="3">
         <f t="shared" si="12"/>
         <v>2.5132741228718345</v>
       </c>
+      <c r="H43" s="1">
+        <f t="shared" si="13"/>
+        <v>5.6408497187473705E-2</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" si="14"/>
+        <v>2.5132741228718345</v>
+      </c>
       <c r="K43" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.65450849718747361</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M43" s="3">
+        <f t="shared" si="7"/>
+        <v>2.5132741228718345</v>
+      </c>
+      <c r="N43" s="13">
+        <f t="shared" si="8"/>
+        <v>0.15190000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <f t="shared" si="7"/>
-        <v>2.57610597594363</v>
-      </c>
-      <c r="B44" s="1">
-        <f t="shared" si="8"/>
-        <v>7.7836037248992601E-2</v>
-      </c>
-      <c r="D44" s="3">
         <f t="shared" si="9"/>
         <v>2.57610597594363</v>
       </c>
+      <c r="B44" s="1">
+        <f t="shared" si="10"/>
+        <v>7.7836037248992601E-2</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="11"/>
+        <v>2.57610597594363</v>
+      </c>
       <c r="E44" s="1">
         <v>0.13134999999999999</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" si="10"/>
-        <v>2.57610597594363</v>
-      </c>
-      <c r="H44" s="1">
-        <f t="shared" si="11"/>
-        <v>5.3513962751007393E-2</v>
-      </c>
-      <c r="J44" s="3">
         <f t="shared" si="12"/>
         <v>2.57610597594363</v>
       </c>
+      <c r="H44" s="1">
+        <f t="shared" si="13"/>
+        <v>5.3513962751007393E-2</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" si="14"/>
+        <v>2.57610597594363</v>
+      </c>
       <c r="K44" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.712889645782536</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M44" s="3">
+        <f t="shared" si="7"/>
+        <v>2.57610597594363</v>
+      </c>
+      <c r="N44" s="13">
+        <f t="shared" si="8"/>
+        <v>0.13139999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <f t="shared" si="7"/>
-        <v>2.6389378290154264</v>
-      </c>
-      <c r="B45" s="1">
-        <f t="shared" si="8"/>
-        <v>6.184665997806818E-2</v>
-      </c>
-      <c r="D45" s="3">
         <f t="shared" si="9"/>
         <v>2.6389378290154264</v>
       </c>
+      <c r="B45" s="1">
+        <f t="shared" si="10"/>
+        <v>6.184665997806818E-2</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="11"/>
+        <v>2.6389378290154264</v>
+      </c>
       <c r="E45" s="1">
         <v>0.1208</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" si="10"/>
-        <v>2.6389378290154264</v>
-      </c>
-      <c r="H45" s="1">
-        <f t="shared" si="11"/>
-        <v>5.8953340021931824E-2</v>
-      </c>
-      <c r="J45" s="3">
         <f t="shared" si="12"/>
         <v>2.6389378290154264</v>
       </c>
+      <c r="H45" s="1">
+        <f t="shared" si="13"/>
+        <v>5.8953340021931824E-2</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="14"/>
+        <v>2.6389378290154264</v>
+      </c>
       <c r="K45" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.76791339748949827</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M45" s="3">
+        <f t="shared" si="7"/>
+        <v>2.6389378290154264</v>
+      </c>
+      <c r="N45" s="13">
+        <f t="shared" si="8"/>
+        <v>0.1208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <f t="shared" si="7"/>
-        <v>2.7017696820872219</v>
-      </c>
-      <c r="B46" s="1">
-        <f t="shared" si="8"/>
-        <v>4.7586473766990302E-2</v>
-      </c>
-      <c r="D46" s="3">
         <f t="shared" si="9"/>
         <v>2.7017696820872219</v>
       </c>
+      <c r="B46" s="1">
+        <f t="shared" si="10"/>
+        <v>4.7586473766990302E-2</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="11"/>
+        <v>2.7017696820872219</v>
+      </c>
       <c r="E46" s="1">
         <v>0.1051</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" si="10"/>
-        <v>2.7017696820872219</v>
-      </c>
-      <c r="H46" s="1">
-        <f t="shared" si="11"/>
-        <v>5.7513526233009697E-2</v>
-      </c>
-      <c r="J46" s="3">
         <f t="shared" si="12"/>
         <v>2.7017696820872219</v>
       </c>
+      <c r="H46" s="1">
+        <f t="shared" si="13"/>
+        <v>5.7513526233009697E-2</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="14"/>
+        <v>2.7017696820872219</v>
+      </c>
       <c r="K46" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.81871199487434454</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M46" s="3">
+        <f t="shared" si="7"/>
+        <v>2.7017696820872219</v>
+      </c>
+      <c r="N46" s="13">
+        <f t="shared" si="8"/>
+        <v>0.1051</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <f t="shared" si="7"/>
-        <v>2.7646015351590179</v>
-      </c>
-      <c r="B47" s="1">
-        <f t="shared" si="8"/>
-        <v>3.511175705587434E-2</v>
-      </c>
-      <c r="D47" s="3">
         <f t="shared" si="9"/>
         <v>2.7646015351590179</v>
       </c>
+      <c r="B47" s="1">
+        <f t="shared" si="10"/>
+        <v>3.511175705587434E-2</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="11"/>
+        <v>2.7646015351590179</v>
+      </c>
       <c r="E47" s="1">
         <v>9.7250000000000003E-2</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" si="10"/>
-        <v>2.7646015351590179</v>
-      </c>
-      <c r="H47" s="1">
-        <f t="shared" si="11"/>
-        <v>6.2138242944125663E-2</v>
-      </c>
-      <c r="J47" s="3">
         <f t="shared" si="12"/>
         <v>2.7646015351590179</v>
       </c>
+      <c r="H47" s="1">
+        <f t="shared" si="13"/>
+        <v>6.2138242944125663E-2</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="14"/>
+        <v>2.7646015351590179</v>
+      </c>
       <c r="K47" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.86448431371070567</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M47" s="3">
+        <f t="shared" si="7"/>
+        <v>2.7646015351590179</v>
+      </c>
+      <c r="N47" s="13">
+        <f t="shared" si="8"/>
+        <v>9.7199999999999995E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <f t="shared" si="7"/>
-        <v>2.8274333882308138</v>
-      </c>
-      <c r="B48" s="1">
-        <f t="shared" si="8"/>
-        <v>2.4471741852423231E-2</v>
-      </c>
-      <c r="D48" s="3">
         <f t="shared" si="9"/>
         <v>2.8274333882308138</v>
       </c>
+      <c r="B48" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4471741852423231E-2</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="11"/>
+        <v>2.8274333882308138</v>
+      </c>
       <c r="E48" s="1">
         <v>7.9100000000000004E-2</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" si="10"/>
-        <v>2.8274333882308138</v>
-      </c>
-      <c r="H48" s="1">
-        <f t="shared" si="11"/>
-        <v>5.4628258147576769E-2</v>
-      </c>
-      <c r="J48" s="3">
         <f t="shared" si="12"/>
         <v>2.8274333882308138</v>
       </c>
+      <c r="H48" s="1">
+        <f t="shared" si="13"/>
+        <v>5.4628258147576769E-2</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="14"/>
+        <v>2.8274333882308138</v>
+      </c>
       <c r="K48" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.90450849718747361</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M48" s="3">
+        <f t="shared" si="7"/>
+        <v>2.8274333882308138</v>
+      </c>
+      <c r="N48" s="13">
+        <f t="shared" si="8"/>
+        <v>7.9100000000000004E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <f t="shared" si="7"/>
-        <v>2.8902652413026093</v>
-      </c>
-      <c r="B49" s="1">
-        <f t="shared" si="8"/>
-        <v>1.57084194356845E-2</v>
-      </c>
-      <c r="D49" s="3">
         <f t="shared" si="9"/>
         <v>2.8902652413026093</v>
       </c>
+      <c r="B49" s="1">
+        <f t="shared" si="10"/>
+        <v>1.57084194356845E-2</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="11"/>
+        <v>2.8902652413026093</v>
+      </c>
       <c r="E49" s="1">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="G49" s="3">
-        <f t="shared" si="10"/>
-        <v>2.8902652413026093</v>
-      </c>
-      <c r="H49" s="1">
-        <f t="shared" si="11"/>
-        <v>6.0291580564315495E-2</v>
-      </c>
-      <c r="J49" s="3">
         <f t="shared" si="12"/>
         <v>2.8902652413026093</v>
       </c>
+      <c r="H49" s="1">
+        <f t="shared" si="13"/>
+        <v>6.0291580564315495E-2</v>
+      </c>
+      <c r="J49" s="3">
+        <f t="shared" si="14"/>
+        <v>2.8902652413026093</v>
+      </c>
       <c r="K49" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.93815334002193151</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M49" s="3">
+        <f t="shared" si="7"/>
+        <v>2.8902652413026093</v>
+      </c>
+      <c r="N49" s="13">
+        <f t="shared" si="8"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <f t="shared" si="7"/>
-        <v>2.9530970943744057</v>
-      </c>
-      <c r="B50" s="1">
-        <f t="shared" si="8"/>
-        <v>8.8563746356556533E-3</v>
-      </c>
-      <c r="D50" s="3">
         <f t="shared" si="9"/>
         <v>2.9530970943744057</v>
       </c>
+      <c r="B50" s="1">
+        <f t="shared" si="10"/>
+        <v>8.8563746356556533E-3</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="11"/>
+        <v>2.9530970943744057</v>
+      </c>
       <c r="E50" s="1">
         <v>6.8900000000000003E-2</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="10"/>
-        <v>2.9530970943744057</v>
-      </c>
-      <c r="H50" s="1">
-        <f t="shared" si="11"/>
-        <v>6.004362536434435E-2</v>
-      </c>
-      <c r="J50" s="3">
         <f t="shared" si="12"/>
         <v>2.9530970943744057</v>
       </c>
+      <c r="H50" s="1">
+        <f t="shared" si="13"/>
+        <v>6.004362536434435E-2</v>
+      </c>
+      <c r="J50" s="3">
+        <f t="shared" si="14"/>
+        <v>2.9530970943744057</v>
+      </c>
       <c r="K50" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.96488824294412578</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M50" s="3">
+        <f t="shared" si="7"/>
+        <v>2.9530970943744057</v>
+      </c>
+      <c r="N50" s="13">
+        <f t="shared" si="8"/>
+        <v>6.8900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <f t="shared" si="7"/>
-        <v>3.0159289474462012</v>
-      </c>
-      <c r="B51" s="1">
-        <f t="shared" si="8"/>
-        <v>3.9426493427611037E-3</v>
-      </c>
-      <c r="D51" s="3">
         <f t="shared" si="9"/>
         <v>3.0159289474462012</v>
       </c>
+      <c r="B51" s="1">
+        <f t="shared" si="10"/>
+        <v>3.9426493427611037E-3</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="11"/>
+        <v>3.0159289474462012</v>
+      </c>
       <c r="E51" s="1">
         <v>6.3200000000000006E-2</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="10"/>
-        <v>3.0159289474462012</v>
-      </c>
-      <c r="H51" s="1">
-        <f t="shared" si="11"/>
-        <v>5.9257350657238902E-2</v>
-      </c>
-      <c r="J51" s="3">
         <f t="shared" si="12"/>
         <v>3.0159289474462012</v>
       </c>
+      <c r="H51" s="1">
+        <f t="shared" si="13"/>
+        <v>5.9257350657238902E-2</v>
+      </c>
+      <c r="J51" s="3">
+        <f t="shared" si="14"/>
+        <v>3.0159289474462012</v>
+      </c>
       <c r="K51" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.98429158056431543</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M51" s="3">
+        <f t="shared" si="7"/>
+        <v>3.0159289474462012</v>
+      </c>
+      <c r="N51" s="13">
+        <f t="shared" si="8"/>
+        <v>6.3200000000000006E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <f t="shared" si="7"/>
-        <v>3.0787608005179972</v>
-      </c>
-      <c r="B52" s="1">
-        <f t="shared" si="8"/>
-        <v>9.866357858642255E-4</v>
-      </c>
-      <c r="D52" s="3">
         <f t="shared" si="9"/>
         <v>3.0787608005179972</v>
       </c>
+      <c r="B52" s="1">
+        <f t="shared" si="10"/>
+        <v>9.866357858642255E-4</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="11"/>
+        <v>3.0787608005179972</v>
+      </c>
       <c r="E52" s="1">
         <v>0.06</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" si="10"/>
-        <v>3.0787608005179972</v>
-      </c>
-      <c r="H52" s="1">
-        <f t="shared" si="11"/>
-        <v>5.901336421413577E-2</v>
-      </c>
-      <c r="J52" s="3">
         <f t="shared" si="12"/>
         <v>3.0787608005179972</v>
       </c>
+      <c r="H52" s="1">
+        <f t="shared" si="13"/>
+        <v>5.901336421413577E-2</v>
+      </c>
+      <c r="J52" s="3">
+        <f t="shared" si="14"/>
+        <v>3.0787608005179972</v>
+      </c>
       <c r="K52" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99605735065723888</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M52" s="3">
+        <f t="shared" si="7"/>
+        <v>3.0787608005179972</v>
+      </c>
+      <c r="N52" s="13">
+        <f t="shared" si="8"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <f t="shared" si="7"/>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="B53" s="1">
-        <f t="shared" si="8"/>
-        <v>3.7524718414124473E-33</v>
-      </c>
-      <c r="D53" s="3">
         <f t="shared" si="9"/>
         <v>3.1415926535897931</v>
       </c>
+      <c r="B53" s="1">
+        <f t="shared" si="10"/>
+        <v>3.7524718414124473E-33</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="11"/>
+        <v>3.1415926535897931</v>
+      </c>
       <c r="E53" s="1">
         <v>5.4899999999999997E-2</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.1415926535897931</v>
       </c>
       <c r="H53" s="1">
@@ -2263,1649 +2679,2049 @@
         <v>5.4899999999999997E-2</v>
       </c>
       <c r="J53" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.1415926535897931</v>
       </c>
       <c r="K53" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M53" s="3">
+        <f t="shared" si="7"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="N53" s="13">
+        <f t="shared" si="8"/>
+        <v>5.4899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <f t="shared" si="7"/>
-        <v>3.2044245066615891</v>
-      </c>
-      <c r="B54" s="1">
-        <f t="shared" si="8"/>
-        <v>9.8663578586421813E-4</v>
-      </c>
-      <c r="D54" s="3">
         <f t="shared" si="9"/>
         <v>3.2044245066615891</v>
       </c>
+      <c r="B54" s="1">
+        <f t="shared" si="10"/>
+        <v>9.8663578586421813E-4</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="11"/>
+        <v>3.2044245066615891</v>
+      </c>
       <c r="E54" s="1">
         <v>6.1650000000000003E-2</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" si="10"/>
-        <v>3.2044245066615891</v>
-      </c>
-      <c r="H54" s="1">
-        <f t="shared" si="11"/>
-        <v>6.0663364214135783E-2</v>
-      </c>
-      <c r="J54" s="3">
         <f t="shared" si="12"/>
         <v>3.2044245066615891</v>
       </c>
+      <c r="H54" s="1">
+        <f t="shared" si="13"/>
+        <v>6.0663364214135783E-2</v>
+      </c>
+      <c r="J54" s="3">
+        <f t="shared" si="14"/>
+        <v>3.2044245066615891</v>
+      </c>
       <c r="K54" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.99605735065723888</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M54" s="3">
+        <f t="shared" si="7"/>
+        <v>3.2044245066615891</v>
+      </c>
+      <c r="N54" s="13">
+        <f t="shared" si="8"/>
+        <v>6.1600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <f t="shared" si="7"/>
-        <v>3.267256359733385</v>
-      </c>
-      <c r="B55" s="1">
-        <f t="shared" si="8"/>
-        <v>3.9426493427610881E-3</v>
-      </c>
-      <c r="D55" s="3">
         <f t="shared" si="9"/>
         <v>3.267256359733385</v>
       </c>
+      <c r="B55" s="1">
+        <f t="shared" si="10"/>
+        <v>3.9426493427610881E-3</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="11"/>
+        <v>3.267256359733385</v>
+      </c>
       <c r="E55" s="1">
         <v>6.275E-2</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="10"/>
-        <v>3.267256359733385</v>
-      </c>
-      <c r="H55" s="1">
-        <f t="shared" si="11"/>
-        <v>5.880735065723891E-2</v>
-      </c>
-      <c r="J55" s="3">
         <f t="shared" si="12"/>
         <v>3.267256359733385</v>
       </c>
+      <c r="H55" s="1">
+        <f t="shared" si="13"/>
+        <v>5.880735065723891E-2</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="14"/>
+        <v>3.267256359733385</v>
+      </c>
       <c r="K55" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.98429158056431565</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M55" s="3">
+        <f t="shared" si="7"/>
+        <v>3.267256359733385</v>
+      </c>
+      <c r="N55" s="13">
+        <f t="shared" si="8"/>
+        <v>6.2799999999999995E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <f t="shared" si="7"/>
-        <v>3.330088212805181</v>
-      </c>
-      <c r="B56" s="1">
-        <f t="shared" si="8"/>
-        <v>8.8563746356556707E-3</v>
-      </c>
-      <c r="D56" s="3">
         <f t="shared" si="9"/>
         <v>3.330088212805181</v>
       </c>
+      <c r="B56" s="1">
+        <f t="shared" si="10"/>
+        <v>8.8563746356556707E-3</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="11"/>
+        <v>3.330088212805181</v>
+      </c>
       <c r="E56" s="1">
         <v>6.5600000000000006E-2</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" si="10"/>
-        <v>3.330088212805181</v>
-      </c>
-      <c r="H56" s="1">
-        <f t="shared" si="11"/>
-        <v>5.6743625364344338E-2</v>
-      </c>
-      <c r="J56" s="3">
         <f t="shared" si="12"/>
         <v>3.330088212805181</v>
       </c>
+      <c r="H56" s="1">
+        <f t="shared" si="13"/>
+        <v>5.6743625364344338E-2</v>
+      </c>
+      <c r="J56" s="3">
+        <f t="shared" si="14"/>
+        <v>3.330088212805181</v>
+      </c>
       <c r="K56" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.96488824294412556</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M56" s="3">
+        <f t="shared" si="7"/>
+        <v>3.330088212805181</v>
+      </c>
+      <c r="N56" s="13">
+        <f t="shared" si="8"/>
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <f t="shared" si="7"/>
-        <v>3.3929200658769765</v>
-      </c>
-      <c r="B57" s="1">
-        <f t="shared" si="8"/>
-        <v>1.5708419435684417E-2</v>
-      </c>
-      <c r="D57" s="3">
         <f t="shared" si="9"/>
         <v>3.3929200658769765</v>
       </c>
+      <c r="B57" s="1">
+        <f t="shared" si="10"/>
+        <v>1.5708419435684417E-2</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="11"/>
+        <v>3.3929200658769765</v>
+      </c>
       <c r="E57" s="1">
         <v>7.0599999999999996E-2</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" si="10"/>
-        <v>3.3929200658769765</v>
-      </c>
-      <c r="H57" s="1">
-        <f t="shared" si="11"/>
-        <v>5.4891580564315576E-2</v>
-      </c>
-      <c r="J57" s="3">
         <f t="shared" si="12"/>
         <v>3.3929200658769765</v>
       </c>
+      <c r="H57" s="1">
+        <f t="shared" si="13"/>
+        <v>5.4891580564315576E-2</v>
+      </c>
+      <c r="J57" s="3">
+        <f t="shared" si="14"/>
+        <v>3.3929200658769765</v>
+      </c>
       <c r="K57" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.93815334002193196</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M57" s="3">
+        <f t="shared" si="7"/>
+        <v>3.3929200658769765</v>
+      </c>
+      <c r="N57" s="13">
+        <f t="shared" si="8"/>
+        <v>7.0599999999999996E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <f t="shared" si="7"/>
-        <v>3.4557519189487724</v>
-      </c>
-      <c r="B58" s="1">
-        <f t="shared" si="8"/>
-        <v>2.4471741852423196E-2</v>
-      </c>
-      <c r="D58" s="3">
         <f t="shared" si="9"/>
         <v>3.4557519189487724</v>
       </c>
+      <c r="B58" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4471741852423196E-2</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="11"/>
+        <v>3.4557519189487724</v>
+      </c>
       <c r="E58" s="1">
         <v>8.43E-2</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" si="10"/>
-        <v>3.4557519189487724</v>
-      </c>
-      <c r="H58" s="1">
-        <f t="shared" si="11"/>
-        <v>5.9828258147576807E-2</v>
-      </c>
-      <c r="J58" s="3">
         <f t="shared" si="12"/>
         <v>3.4557519189487724</v>
       </c>
+      <c r="H58" s="1">
+        <f t="shared" si="13"/>
+        <v>5.9828258147576807E-2</v>
+      </c>
+      <c r="J58" s="3">
+        <f t="shared" si="14"/>
+        <v>3.4557519189487724</v>
+      </c>
       <c r="K58" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.90450849718747384</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M58" s="3">
+        <f t="shared" si="7"/>
+        <v>3.4557519189487724</v>
+      </c>
+      <c r="N58" s="13">
+        <f t="shared" si="8"/>
+        <v>8.43E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <f t="shared" si="7"/>
-        <v>3.5185837720205684</v>
-      </c>
-      <c r="B59" s="1">
-        <f t="shared" si="8"/>
-        <v>3.5111757055874285E-2</v>
-      </c>
-      <c r="D59" s="3">
         <f t="shared" si="9"/>
         <v>3.5185837720205684</v>
       </c>
+      <c r="B59" s="1">
+        <f t="shared" si="10"/>
+        <v>3.5111757055874285E-2</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="11"/>
+        <v>3.5185837720205684</v>
+      </c>
       <c r="E59" s="1">
         <v>9.3850000000000003E-2</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" si="10"/>
-        <v>3.5185837720205684</v>
-      </c>
-      <c r="H59" s="1">
-        <f t="shared" si="11"/>
-        <v>5.8738242944125718E-2</v>
-      </c>
-      <c r="J59" s="3">
         <f t="shared" si="12"/>
         <v>3.5185837720205684</v>
       </c>
+      <c r="H59" s="1">
+        <f t="shared" si="13"/>
+        <v>5.8738242944125718E-2</v>
+      </c>
+      <c r="J59" s="3">
+        <f t="shared" si="14"/>
+        <v>3.5185837720205684</v>
+      </c>
       <c r="K59" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.86448431371070589</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M59" s="3">
+        <f t="shared" si="7"/>
+        <v>3.5185837720205684</v>
+      </c>
+      <c r="N59" s="13">
+        <f t="shared" si="8"/>
+        <v>9.3799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <f t="shared" si="7"/>
-        <v>3.5814156250923639</v>
-      </c>
-      <c r="B60" s="1">
-        <f t="shared" si="8"/>
-        <v>4.7586473766990142E-2</v>
-      </c>
-      <c r="D60" s="3">
         <f t="shared" si="9"/>
         <v>3.5814156250923639</v>
       </c>
+      <c r="B60" s="1">
+        <f t="shared" si="10"/>
+        <v>4.7586473766990142E-2</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="11"/>
+        <v>3.5814156250923639</v>
+      </c>
       <c r="E60" s="1">
         <v>9.9699999999999997E-2</v>
       </c>
       <c r="G60" s="3">
-        <f t="shared" si="10"/>
-        <v>3.5814156250923639</v>
-      </c>
-      <c r="H60" s="1">
-        <f t="shared" si="11"/>
-        <v>5.2113526233009855E-2</v>
-      </c>
-      <c r="J60" s="3">
         <f t="shared" si="12"/>
         <v>3.5814156250923639</v>
       </c>
+      <c r="H60" s="1">
+        <f t="shared" si="13"/>
+        <v>5.2113526233009855E-2</v>
+      </c>
+      <c r="J60" s="3">
+        <f t="shared" si="14"/>
+        <v>3.5814156250923639</v>
+      </c>
       <c r="K60" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.81871199487434509</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M60" s="3">
+        <f t="shared" si="7"/>
+        <v>3.5814156250923639</v>
+      </c>
+      <c r="N60" s="13">
+        <f t="shared" si="8"/>
+        <v>9.9699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <f t="shared" si="7"/>
-        <v>3.6442474781641603</v>
-      </c>
-      <c r="B61" s="1">
-        <f t="shared" si="8"/>
-        <v>6.1846659978068236E-2</v>
-      </c>
-      <c r="D61" s="3">
         <f t="shared" si="9"/>
         <v>3.6442474781641603</v>
       </c>
+      <c r="B61" s="1">
+        <f t="shared" si="10"/>
+        <v>6.1846659978068236E-2</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="11"/>
+        <v>3.6442474781641603</v>
+      </c>
       <c r="E61" s="1">
         <v>0.11575000000000001</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" si="10"/>
-        <v>3.6442474781641603</v>
-      </c>
-      <c r="H61" s="1">
-        <f t="shared" si="11"/>
-        <v>5.390334002193177E-2</v>
-      </c>
-      <c r="J61" s="3">
         <f t="shared" si="12"/>
         <v>3.6442474781641603</v>
       </c>
+      <c r="H61" s="1">
+        <f t="shared" si="13"/>
+        <v>5.390334002193177E-2</v>
+      </c>
+      <c r="J61" s="3">
+        <f t="shared" si="14"/>
+        <v>3.6442474781641603</v>
+      </c>
       <c r="K61" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.76791339748949816</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M61" s="3">
+        <f t="shared" si="7"/>
+        <v>3.6442474781641603</v>
+      </c>
+      <c r="N61" s="13">
+        <f t="shared" si="8"/>
+        <v>0.1158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <f t="shared" si="7"/>
-        <v>3.7070793312359558</v>
-      </c>
-      <c r="B62" s="1">
-        <f t="shared" si="8"/>
-        <v>7.7836037248992407E-2</v>
-      </c>
-      <c r="D62" s="3">
         <f t="shared" si="9"/>
         <v>3.7070793312359558</v>
       </c>
+      <c r="B62" s="1">
+        <f t="shared" si="10"/>
+        <v>7.7836037248992407E-2</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="11"/>
+        <v>3.7070793312359558</v>
+      </c>
       <c r="E62" s="1">
         <v>0.12909999999999999</v>
       </c>
       <c r="G62" s="3">
-        <f t="shared" si="10"/>
-        <v>3.7070793312359558</v>
-      </c>
-      <c r="H62" s="1">
-        <f t="shared" si="11"/>
-        <v>5.1263962751007586E-2</v>
-      </c>
-      <c r="J62" s="3">
         <f t="shared" si="12"/>
         <v>3.7070793312359558</v>
       </c>
+      <c r="H62" s="1">
+        <f t="shared" si="13"/>
+        <v>5.1263962751007586E-2</v>
+      </c>
+      <c r="J62" s="3">
+        <f t="shared" si="14"/>
+        <v>3.7070793312359558</v>
+      </c>
       <c r="K62" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.71288964578253655</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M62" s="3">
+        <f t="shared" si="7"/>
+        <v>3.7070793312359558</v>
+      </c>
+      <c r="N62" s="13">
+        <f t="shared" si="8"/>
+        <v>0.12909999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <f t="shared" si="7"/>
-        <v>3.7699111843077513</v>
-      </c>
-      <c r="B63" s="1">
-        <f t="shared" si="8"/>
-        <v>9.5491502812526094E-2</v>
-      </c>
-      <c r="D63" s="3">
         <f t="shared" si="9"/>
         <v>3.7699111843077513</v>
       </c>
+      <c r="B63" s="1">
+        <f t="shared" si="10"/>
+        <v>9.5491502812526094E-2</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="11"/>
+        <v>3.7699111843077513</v>
+      </c>
       <c r="E63" s="1">
         <v>0.1479</v>
       </c>
       <c r="G63" s="3">
-        <f t="shared" si="10"/>
-        <v>3.7699111843077513</v>
-      </c>
-      <c r="H63" s="1">
-        <f t="shared" si="11"/>
-        <v>5.240849718747391E-2</v>
-      </c>
-      <c r="J63" s="3">
         <f t="shared" si="12"/>
         <v>3.7699111843077513</v>
       </c>
+      <c r="H63" s="1">
+        <f t="shared" si="13"/>
+        <v>5.240849718747391E-2</v>
+      </c>
+      <c r="J63" s="3">
+        <f t="shared" si="14"/>
+        <v>3.7699111843077513</v>
+      </c>
       <c r="K63" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.65450849718747428</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M63" s="3">
+        <f t="shared" si="7"/>
+        <v>3.7699111843077513</v>
+      </c>
+      <c r="N63" s="13">
+        <f t="shared" si="8"/>
+        <v>0.1479</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <f t="shared" si="7"/>
-        <v>3.8327430373795477</v>
-      </c>
-      <c r="B64" s="1">
-        <f t="shared" si="8"/>
-        <v>0.11474337861210537</v>
-      </c>
-      <c r="D64" s="3">
         <f t="shared" si="9"/>
         <v>3.8327430373795477</v>
       </c>
+      <c r="B64" s="1">
+        <f t="shared" si="10"/>
+        <v>0.11474337861210537</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="11"/>
+        <v>3.8327430373795477</v>
+      </c>
       <c r="E64" s="1">
         <v>0.16114999999999999</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="10"/>
-        <v>3.8327430373795477</v>
-      </c>
-      <c r="H64" s="1">
-        <f t="shared" si="11"/>
-        <v>4.6406621387894614E-2</v>
-      </c>
-      <c r="J64" s="3">
         <f t="shared" si="12"/>
         <v>3.8327430373795477</v>
       </c>
+      <c r="H64" s="1">
+        <f t="shared" si="13"/>
+        <v>4.6406621387894614E-2</v>
+      </c>
+      <c r="J64" s="3">
+        <f t="shared" si="14"/>
+        <v>3.8327430373795477</v>
+      </c>
       <c r="K64" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.5936906572928623</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M64" s="3">
+        <f t="shared" si="7"/>
+        <v>3.8327430373795477</v>
+      </c>
+      <c r="N64" s="13">
+        <f t="shared" si="8"/>
+        <v>0.16120000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <f t="shared" si="7"/>
-        <v>3.8955748904513432</v>
-      </c>
-      <c r="B65" s="1">
-        <f t="shared" si="8"/>
-        <v>0.13551568628929408</v>
-      </c>
-      <c r="D65" s="3">
         <f t="shared" si="9"/>
         <v>3.8955748904513432</v>
       </c>
+      <c r="B65" s="1">
+        <f t="shared" si="10"/>
+        <v>0.13551568628929408</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="11"/>
+        <v>3.8955748904513432</v>
+      </c>
       <c r="E65" s="1">
         <v>0.1852</v>
       </c>
       <c r="G65" s="3">
-        <f t="shared" si="10"/>
-        <v>3.8955748904513432</v>
-      </c>
-      <c r="H65" s="1">
-        <f t="shared" si="11"/>
-        <v>4.9684313710705919E-2</v>
-      </c>
-      <c r="J65" s="3">
         <f t="shared" si="12"/>
         <v>3.8955748904513432</v>
       </c>
+      <c r="H65" s="1">
+        <f t="shared" si="13"/>
+        <v>4.9684313710705919E-2</v>
+      </c>
+      <c r="J65" s="3">
+        <f t="shared" si="14"/>
+        <v>3.8955748904513432</v>
+      </c>
       <c r="K65" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.53139525976465707</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M65" s="3">
+        <f t="shared" si="7"/>
+        <v>3.8955748904513432</v>
+      </c>
+      <c r="N65" s="13">
+        <f t="shared" si="8"/>
+        <v>0.1852</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <f t="shared" si="7"/>
-        <v>3.9584067435231396</v>
-      </c>
-      <c r="B66" s="1">
-        <f t="shared" si="8"/>
-        <v>0.15772644703565572</v>
-      </c>
-      <c r="D66" s="3">
         <f t="shared" si="9"/>
         <v>3.9584067435231396</v>
       </c>
+      <c r="B66" s="1">
+        <f t="shared" si="10"/>
+        <v>0.15772644703565572</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="11"/>
+        <v>3.9584067435231396</v>
+      </c>
       <c r="E66" s="1">
         <v>0.20485</v>
       </c>
       <c r="G66" s="3">
-        <f t="shared" si="10"/>
-        <v>3.9584067435231396</v>
-      </c>
-      <c r="H66" s="1">
-        <f t="shared" si="11"/>
-        <v>4.7123552964344284E-2</v>
-      </c>
-      <c r="J66" s="3">
         <f t="shared" si="12"/>
         <v>3.9584067435231396</v>
       </c>
+      <c r="H66" s="1">
+        <f t="shared" si="13"/>
+        <v>4.7123552964344284E-2</v>
+      </c>
+      <c r="J66" s="3">
+        <f t="shared" si="14"/>
+        <v>3.9584067435231396</v>
+      </c>
       <c r="K66" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.46860474023534321</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M66" s="3">
+        <f t="shared" si="7"/>
+        <v>3.9584067435231396</v>
+      </c>
+      <c r="N66" s="13">
+        <f t="shared" si="8"/>
+        <v>0.20480000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <f t="shared" ref="A67:A103" si="14">(ROW(A67)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="A67:A103" si="16">(ROW(A67)-ROW($A$3))*PI()/50</f>
         <v>4.0212385965949355</v>
       </c>
       <c r="B67" s="1">
-        <f t="shared" ref="B67:B98" si="15">ABS(COS(A67/2))^2</f>
+        <f t="shared" ref="B67:B98" si="17">ABS(COS(A67/2))^2</f>
         <v>0.18128800512565521</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" ref="D67:D103" si="16">(ROW(D67)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="D67:D103" si="18">(ROW(D67)-ROW($A$3))*PI()/50</f>
         <v>4.0212385965949355</v>
       </c>
       <c r="E67" s="1">
         <v>0.22384999999999999</v>
       </c>
       <c r="G67" s="3">
-        <f t="shared" ref="G67:G103" si="17">(ROW(G67)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="G67:G103" si="19">(ROW(G67)-ROW($A$3))*PI()/50</f>
         <v>4.0212385965949355</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" ref="H67:H102" si="18">ABS(B67-E67)</f>
+        <f t="shared" ref="H67:H102" si="20">ABS(B67-E67)</f>
         <v>4.2561994874344783E-2</v>
       </c>
       <c r="J67" s="3">
-        <f t="shared" ref="J67:J103" si="19">(ROW(J67)-ROW($A$3))*PI()/50</f>
+        <f t="shared" ref="J67:J103" si="21">(ROW(J67)-ROW($A$3))*PI()/50</f>
         <v>4.0212385965949355</v>
       </c>
       <c r="K67" s="1">
-        <f t="shared" ref="K67:K98" si="20">ABS(COS(J67))^2</f>
+        <f t="shared" ref="K67:K98" si="22">ABS(COS(J67))^2</f>
         <v>0.40630934270713742</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M67" s="3">
+        <f t="shared" ref="M67:M103" si="23">(ROW(M67)-ROW($A$3))*PI()/50</f>
+        <v>4.0212385965949355</v>
+      </c>
+      <c r="N67" s="13">
+        <f t="shared" si="8"/>
+        <v>0.2238</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <f t="shared" si="14"/>
-        <v>4.0840704496667311</v>
-      </c>
-      <c r="B68" s="1">
-        <f t="shared" si="15"/>
-        <v>0.20610737385376335</v>
-      </c>
-      <c r="D68" s="3">
         <f t="shared" si="16"/>
         <v>4.0840704496667311</v>
       </c>
+      <c r="B68" s="1">
+        <f t="shared" si="17"/>
+        <v>0.20610737385376335</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="18"/>
+        <v>4.0840704496667311</v>
+      </c>
       <c r="E68" s="1">
         <v>0.24725</v>
       </c>
       <c r="G68" s="3">
-        <f t="shared" si="17"/>
-        <v>4.0840704496667311</v>
-      </c>
-      <c r="H68" s="1">
-        <f t="shared" si="18"/>
-        <v>4.1142626146236649E-2</v>
-      </c>
-      <c r="J68" s="3">
         <f t="shared" si="19"/>
         <v>4.0840704496667311</v>
       </c>
+      <c r="H68" s="1">
+        <f t="shared" si="20"/>
+        <v>4.1142626146236649E-2</v>
+      </c>
+      <c r="J68" s="3">
+        <f t="shared" si="21"/>
+        <v>4.0840704496667311</v>
+      </c>
       <c r="K68" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.34549150281252644</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M68" s="3">
+        <f t="shared" si="23"/>
+        <v>4.0840704496667311</v>
+      </c>
+      <c r="N68" s="13">
+        <f t="shared" ref="N68:N103" si="24">IF(AND(ISEVEN(ROUNDDOWN(E68*10000,1)),ROUNDDOWN(E68*10000,1)&gt;=E68*10000),ROUNDDOWN(E68,4),ROUND(E68,4))</f>
+        <v>0.2472</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <f t="shared" si="14"/>
-        <v>4.1469023027385274</v>
-      </c>
-      <c r="B69" s="1">
-        <f t="shared" si="15"/>
-        <v>0.23208660251050184</v>
-      </c>
-      <c r="D69" s="3">
         <f t="shared" si="16"/>
         <v>4.1469023027385274</v>
       </c>
+      <c r="B69" s="1">
+        <f t="shared" si="17"/>
+        <v>0.23208660251050184</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="18"/>
+        <v>4.1469023027385274</v>
+      </c>
       <c r="E69" s="1">
         <v>0.27174999999999999</v>
       </c>
       <c r="G69" s="3">
-        <f t="shared" si="17"/>
-        <v>4.1469023027385274</v>
-      </c>
-      <c r="H69" s="1">
-        <f t="shared" si="18"/>
-        <v>3.9663397489498153E-2</v>
-      </c>
-      <c r="J69" s="3">
         <f t="shared" si="19"/>
         <v>4.1469023027385274</v>
       </c>
+      <c r="H69" s="1">
+        <f t="shared" si="20"/>
+        <v>3.9663397489498153E-2</v>
+      </c>
+      <c r="J69" s="3">
+        <f t="shared" si="21"/>
+        <v>4.1469023027385274</v>
+      </c>
       <c r="K69" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.28711035421746334</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M69" s="3">
+        <f t="shared" si="23"/>
+        <v>4.1469023027385274</v>
+      </c>
+      <c r="N69" s="13">
+        <f t="shared" si="24"/>
+        <v>0.27179999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <f t="shared" si="14"/>
-        <v>4.209734155810323</v>
-      </c>
-      <c r="B70" s="1">
-        <f t="shared" si="15"/>
-        <v>0.25912316294914239</v>
-      </c>
-      <c r="D70" s="3">
         <f t="shared" si="16"/>
         <v>4.209734155810323</v>
       </c>
+      <c r="B70" s="1">
+        <f t="shared" si="17"/>
+        <v>0.25912316294914239</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="18"/>
+        <v>4.209734155810323</v>
+      </c>
       <c r="E70" s="1">
         <v>0.29780000000000001</v>
       </c>
       <c r="G70" s="3">
-        <f t="shared" si="17"/>
-        <v>4.209734155810323</v>
-      </c>
-      <c r="H70" s="1">
-        <f t="shared" si="18"/>
-        <v>3.8676837050857615E-2</v>
-      </c>
-      <c r="J70" s="3">
         <f t="shared" si="19"/>
         <v>4.209734155810323</v>
       </c>
+      <c r="H70" s="1">
+        <f t="shared" si="20"/>
+        <v>3.8676837050857615E-2</v>
+      </c>
+      <c r="J70" s="3">
+        <f t="shared" si="21"/>
+        <v>4.209734155810323</v>
+      </c>
       <c r="K70" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.23208660251050167</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M70" s="3">
+        <f t="shared" si="23"/>
+        <v>4.209734155810323</v>
+      </c>
+      <c r="N70" s="13">
+        <f t="shared" si="24"/>
+        <v>0.29780000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <f t="shared" si="14"/>
-        <v>4.2725660088821193</v>
-      </c>
-      <c r="B71" s="1">
-        <f t="shared" si="15"/>
-        <v>0.28711035421746395</v>
-      </c>
-      <c r="D71" s="3">
         <f t="shared" si="16"/>
         <v>4.2725660088821193</v>
       </c>
+      <c r="B71" s="1">
+        <f t="shared" si="17"/>
+        <v>0.28711035421746395</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="18"/>
+        <v>4.2725660088821193</v>
+      </c>
       <c r="E71" s="1">
         <v>0.3196</v>
       </c>
       <c r="G71" s="3">
-        <f t="shared" si="17"/>
-        <v>4.2725660088821193</v>
-      </c>
-      <c r="H71" s="1">
-        <f t="shared" si="18"/>
-        <v>3.2489645782536047E-2</v>
-      </c>
-      <c r="J71" s="3">
         <f t="shared" si="19"/>
         <v>4.2725660088821193</v>
       </c>
+      <c r="H71" s="1">
+        <f t="shared" si="20"/>
+        <v>3.2489645782536047E-2</v>
+      </c>
+      <c r="J71" s="3">
+        <f t="shared" si="21"/>
+        <v>4.2725660088821193</v>
+      </c>
       <c r="K71" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.18128800512565474</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M71" s="3">
+        <f t="shared" si="23"/>
+        <v>4.2725660088821193</v>
+      </c>
+      <c r="N71" s="13">
+        <f t="shared" si="24"/>
+        <v>0.3196</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <f t="shared" si="14"/>
-        <v>4.3353978619539149</v>
-      </c>
-      <c r="B72" s="1">
-        <f t="shared" si="15"/>
-        <v>0.31593772365766115</v>
-      </c>
-      <c r="D72" s="3">
         <f t="shared" si="16"/>
         <v>4.3353978619539149</v>
       </c>
+      <c r="B72" s="1">
+        <f t="shared" si="17"/>
+        <v>0.31593772365766115</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="18"/>
+        <v>4.3353978619539149</v>
+      </c>
       <c r="E72" s="1">
         <v>0.34699999999999998</v>
       </c>
       <c r="G72" s="3">
-        <f t="shared" si="17"/>
-        <v>4.3353978619539149</v>
-      </c>
-      <c r="H72" s="1">
-        <f t="shared" si="18"/>
-        <v>3.1062276342338824E-2</v>
-      </c>
-      <c r="J72" s="3">
         <f t="shared" si="19"/>
         <v>4.3353978619539149</v>
       </c>
+      <c r="H72" s="1">
+        <f t="shared" si="20"/>
+        <v>3.1062276342338824E-2</v>
+      </c>
+      <c r="J72" s="3">
+        <f t="shared" si="21"/>
+        <v>4.3353978619539149</v>
+      </c>
       <c r="K72" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.13551568628929414</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M72" s="3">
+        <f t="shared" si="23"/>
+        <v>4.3353978619539149</v>
+      </c>
+      <c r="N72" s="13">
+        <f t="shared" si="24"/>
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <f t="shared" si="14"/>
-        <v>4.3982297150257104</v>
-      </c>
-      <c r="B73" s="1">
-        <f t="shared" si="15"/>
-        <v>0.34549150281252616</v>
-      </c>
-      <c r="D73" s="3">
         <f t="shared" si="16"/>
         <v>4.3982297150257104</v>
       </c>
+      <c r="B73" s="1">
+        <f t="shared" si="17"/>
+        <v>0.34549150281252616</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="18"/>
+        <v>4.3982297150257104</v>
+      </c>
       <c r="E73" s="1">
         <v>0.37075000000000002</v>
       </c>
       <c r="G73" s="3">
-        <f t="shared" si="17"/>
-        <v>4.3982297150257104</v>
-      </c>
-      <c r="H73" s="1">
-        <f t="shared" si="18"/>
-        <v>2.5258497187473861E-2</v>
-      </c>
-      <c r="J73" s="3">
         <f t="shared" si="19"/>
         <v>4.3982297150257104</v>
       </c>
+      <c r="H73" s="1">
+        <f t="shared" si="20"/>
+        <v>2.5258497187473861E-2</v>
+      </c>
+      <c r="J73" s="3">
+        <f t="shared" si="21"/>
+        <v>4.3982297150257104</v>
+      </c>
       <c r="K73" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.5491502812526372E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M73" s="3">
+        <f t="shared" si="23"/>
+        <v>4.3982297150257104</v>
+      </c>
+      <c r="N73" s="13">
+        <f t="shared" si="24"/>
+        <v>0.37080000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <f t="shared" si="14"/>
-        <v>4.4610615680975068</v>
-      </c>
-      <c r="B74" s="1">
-        <f t="shared" si="15"/>
-        <v>0.37565505641757274</v>
-      </c>
-      <c r="D74" s="3">
         <f t="shared" si="16"/>
         <v>4.4610615680975068</v>
       </c>
+      <c r="B74" s="1">
+        <f t="shared" si="17"/>
+        <v>0.37565505641757274</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="18"/>
+        <v>4.4610615680975068</v>
+      </c>
       <c r="E74" s="1">
         <v>0.40289999999999998</v>
       </c>
       <c r="G74" s="3">
-        <f t="shared" si="17"/>
-        <v>4.4610615680975068</v>
-      </c>
-      <c r="H74" s="1">
-        <f t="shared" si="18"/>
-        <v>2.7244943582427239E-2</v>
-      </c>
-      <c r="J74" s="3">
         <f t="shared" si="19"/>
         <v>4.4610615680975068</v>
       </c>
+      <c r="H74" s="1">
+        <f t="shared" si="20"/>
+        <v>2.7244943582427239E-2</v>
+      </c>
+      <c r="J74" s="3">
+        <f t="shared" si="21"/>
+        <v>4.4610615680975068</v>
+      </c>
       <c r="K74" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>6.1846659978068028E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M74" s="3">
+        <f t="shared" si="23"/>
+        <v>4.4610615680975068</v>
+      </c>
+      <c r="N74" s="13">
+        <f t="shared" si="24"/>
+        <v>0.40289999999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <f t="shared" si="14"/>
-        <v>4.5238934211693023</v>
-      </c>
-      <c r="B75" s="1">
-        <f t="shared" si="15"/>
-        <v>0.40630934270713776</v>
-      </c>
-      <c r="D75" s="3">
         <f t="shared" si="16"/>
         <v>4.5238934211693023</v>
       </c>
+      <c r="B75" s="1">
+        <f t="shared" si="17"/>
+        <v>0.40630934270713776</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="18"/>
+        <v>4.5238934211693023</v>
+      </c>
       <c r="E75" s="1">
         <v>0.42895</v>
       </c>
       <c r="G75" s="3">
-        <f t="shared" si="17"/>
-        <v>4.5238934211693023</v>
-      </c>
-      <c r="H75" s="1">
-        <f t="shared" si="18"/>
-        <v>2.2640657292862243E-2</v>
-      </c>
-      <c r="J75" s="3">
         <f t="shared" si="19"/>
         <v>4.5238934211693023</v>
       </c>
+      <c r="H75" s="1">
+        <f t="shared" si="20"/>
+        <v>2.2640657292862243E-2</v>
+      </c>
+      <c r="J75" s="3">
+        <f t="shared" si="21"/>
+        <v>4.5238934211693023</v>
+      </c>
       <c r="K75" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.5111757055874299E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M75" s="3">
+        <f t="shared" si="23"/>
+        <v>4.5238934211693023</v>
+      </c>
+      <c r="N75" s="13">
+        <f t="shared" si="24"/>
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <f t="shared" si="14"/>
-        <v>4.5867252742410978</v>
-      </c>
-      <c r="B76" s="1">
-        <f t="shared" si="15"/>
-        <v>0.43733338321784765</v>
-      </c>
-      <c r="D76" s="3">
         <f t="shared" si="16"/>
         <v>4.5867252742410978</v>
       </c>
+      <c r="B76" s="1">
+        <f t="shared" si="17"/>
+        <v>0.43733338321784765</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="18"/>
+        <v>4.5867252742410978</v>
+      </c>
       <c r="E76" s="1">
         <v>0.46534999999999999</v>
       </c>
       <c r="G76" s="3">
-        <f t="shared" si="17"/>
-        <v>4.5867252742410978</v>
-      </c>
-      <c r="H76" s="1">
-        <f t="shared" si="18"/>
-        <v>2.8016616782152337E-2</v>
-      </c>
-      <c r="J76" s="3">
         <f t="shared" si="19"/>
         <v>4.5867252742410978</v>
       </c>
+      <c r="H76" s="1">
+        <f t="shared" si="20"/>
+        <v>2.8016616782152337E-2</v>
+      </c>
+      <c r="J76" s="3">
+        <f t="shared" si="21"/>
+        <v>4.5867252742410978</v>
+      </c>
       <c r="K76" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.5708419435684528E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M76" s="3">
+        <f t="shared" si="23"/>
+        <v>4.5867252742410978</v>
+      </c>
+      <c r="N76" s="13">
+        <f t="shared" si="24"/>
+        <v>0.46539999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <f t="shared" si="14"/>
-        <v>4.6495571273128942</v>
-      </c>
-      <c r="B77" s="1">
-        <f t="shared" si="15"/>
-        <v>0.46860474023534338</v>
-      </c>
-      <c r="D77" s="3">
         <f t="shared" si="16"/>
         <v>4.6495571273128942</v>
       </c>
+      <c r="B77" s="1">
+        <f t="shared" si="17"/>
+        <v>0.46860474023534338</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="18"/>
+        <v>4.6495571273128942</v>
+      </c>
       <c r="E77" s="1">
         <v>0.48885000000000001</v>
       </c>
       <c r="G77" s="3">
-        <f t="shared" si="17"/>
-        <v>4.6495571273128942</v>
-      </c>
-      <c r="H77" s="1">
-        <f t="shared" si="18"/>
-        <v>2.0245259764656631E-2</v>
-      </c>
-      <c r="J77" s="3">
         <f t="shared" si="19"/>
         <v>4.6495571273128942</v>
       </c>
+      <c r="H77" s="1">
+        <f t="shared" si="20"/>
+        <v>2.0245259764656631E-2</v>
+      </c>
+      <c r="J77" s="3">
+        <f t="shared" si="21"/>
+        <v>4.6495571273128942</v>
+      </c>
       <c r="K77" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.9426493427610629E-3</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M77" s="3">
+        <f t="shared" si="23"/>
+        <v>4.6495571273128942</v>
+      </c>
+      <c r="N77" s="13">
+        <f t="shared" si="24"/>
+        <v>0.48880000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <f t="shared" si="14"/>
-        <v>4.7123889803846897</v>
-      </c>
-      <c r="B78" s="1">
-        <f t="shared" si="15"/>
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="D78" s="3">
         <f t="shared" si="16"/>
         <v>4.7123889803846897</v>
       </c>
+      <c r="B78" s="1">
+        <f t="shared" si="17"/>
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="18"/>
+        <v>4.7123889803846897</v>
+      </c>
       <c r="E78" s="1">
         <v>0.52124999999999999</v>
       </c>
       <c r="G78" s="3">
-        <f t="shared" si="17"/>
-        <v>4.7123889803846897</v>
-      </c>
-      <c r="H78" s="1">
-        <f t="shared" si="18"/>
-        <v>2.1250000000000102E-2</v>
-      </c>
-      <c r="J78" s="3">
         <f t="shared" si="19"/>
         <v>4.7123889803846897</v>
       </c>
+      <c r="H78" s="1">
+        <f t="shared" si="20"/>
+        <v>2.1250000000000102E-2</v>
+      </c>
+      <c r="J78" s="3">
+        <f t="shared" si="21"/>
+        <v>4.7123889803846897</v>
+      </c>
       <c r="K78" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.3772246572712026E-32</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M78" s="3">
+        <f t="shared" si="23"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="N78" s="13">
+        <f t="shared" si="24"/>
+        <v>0.5212</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <f t="shared" si="14"/>
-        <v>4.7752208334564852</v>
-      </c>
-      <c r="B79" s="1">
-        <f t="shared" si="15"/>
-        <v>0.5313952597646564</v>
-      </c>
-      <c r="D79" s="3">
         <f t="shared" si="16"/>
         <v>4.7752208334564852</v>
       </c>
+      <c r="B79" s="1">
+        <f t="shared" si="17"/>
+        <v>0.5313952597646564</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="18"/>
+        <v>4.7752208334564852</v>
+      </c>
       <c r="E79" s="1">
         <v>0.54984999999999995</v>
       </c>
       <c r="G79" s="3">
-        <f t="shared" si="17"/>
-        <v>4.7752208334564852</v>
-      </c>
-      <c r="H79" s="1">
-        <f t="shared" si="18"/>
-        <v>1.8454740235343547E-2</v>
-      </c>
-      <c r="J79" s="3">
         <f t="shared" si="19"/>
         <v>4.7752208334564852</v>
       </c>
+      <c r="H79" s="1">
+        <f t="shared" si="20"/>
+        <v>1.8454740235343547E-2</v>
+      </c>
+      <c r="J79" s="3">
+        <f t="shared" si="21"/>
+        <v>4.7752208334564852</v>
+      </c>
       <c r="K79" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.9426493427610161E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M79" s="3">
+        <f t="shared" si="23"/>
+        <v>4.7752208334564852</v>
+      </c>
+      <c r="N79" s="13">
+        <f t="shared" si="24"/>
+        <v>0.54979999999999996</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <f t="shared" si="14"/>
-        <v>4.8380526865282816</v>
-      </c>
-      <c r="B80" s="1">
-        <f t="shared" si="15"/>
-        <v>0.56266661678215224</v>
-      </c>
-      <c r="D80" s="3">
         <f t="shared" si="16"/>
         <v>4.8380526865282816</v>
       </c>
+      <c r="B80" s="1">
+        <f t="shared" si="17"/>
+        <v>0.56266661678215224</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="18"/>
+        <v>4.8380526865282816</v>
+      </c>
       <c r="E80" s="1">
         <v>0.57855000000000001</v>
       </c>
       <c r="G80" s="3">
-        <f t="shared" si="17"/>
-        <v>4.8380526865282816</v>
-      </c>
-      <c r="H80" s="1">
-        <f t="shared" si="18"/>
-        <v>1.5883383217847769E-2</v>
-      </c>
-      <c r="J80" s="3">
         <f t="shared" si="19"/>
         <v>4.8380526865282816</v>
       </c>
+      <c r="H80" s="1">
+        <f t="shared" si="20"/>
+        <v>1.5883383217847769E-2</v>
+      </c>
+      <c r="J80" s="3">
+        <f t="shared" si="21"/>
+        <v>4.8380526865282816</v>
+      </c>
       <c r="K80" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.5708419435684438E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M80" s="3">
+        <f t="shared" si="23"/>
+        <v>4.8380526865282816</v>
+      </c>
+      <c r="N80" s="13">
+        <f t="shared" si="24"/>
+        <v>0.5786</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <f t="shared" si="14"/>
-        <v>4.9008845396000771</v>
-      </c>
-      <c r="B81" s="1">
-        <f t="shared" si="15"/>
-        <v>0.59369065729286219</v>
-      </c>
-      <c r="D81" s="3">
         <f t="shared" si="16"/>
         <v>4.9008845396000771</v>
       </c>
+      <c r="B81" s="1">
+        <f t="shared" si="17"/>
+        <v>0.59369065729286219</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="18"/>
+        <v>4.9008845396000771</v>
+      </c>
       <c r="E81" s="1">
         <v>0.60840000000000005</v>
       </c>
       <c r="G81" s="3">
-        <f t="shared" si="17"/>
-        <v>4.9008845396000771</v>
-      </c>
-      <c r="H81" s="1">
-        <f t="shared" si="18"/>
-        <v>1.4709342707137862E-2</v>
-      </c>
-      <c r="J81" s="3">
         <f t="shared" si="19"/>
         <v>4.9008845396000771</v>
       </c>
+      <c r="H81" s="1">
+        <f t="shared" si="20"/>
+        <v>1.4709342707137862E-2</v>
+      </c>
+      <c r="J81" s="3">
+        <f t="shared" si="21"/>
+        <v>4.9008845396000771</v>
+      </c>
       <c r="K81" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.511175705587416E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M81" s="3">
+        <f t="shared" si="23"/>
+        <v>4.9008845396000771</v>
+      </c>
+      <c r="N81" s="13">
+        <f t="shared" si="24"/>
+        <v>0.60840000000000005</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <f t="shared" si="14"/>
-        <v>4.9637163926718735</v>
-      </c>
-      <c r="B82" s="1">
-        <f t="shared" si="15"/>
-        <v>0.62434494358242743</v>
-      </c>
-      <c r="D82" s="3">
         <f t="shared" si="16"/>
         <v>4.9637163926718735</v>
       </c>
+      <c r="B82" s="1">
+        <f t="shared" si="17"/>
+        <v>0.62434494358242743</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="18"/>
+        <v>4.9637163926718735</v>
+      </c>
       <c r="E82" s="1">
         <v>0.64070000000000005</v>
       </c>
       <c r="G82" s="3">
-        <f t="shared" si="17"/>
-        <v>4.9637163926718735</v>
-      </c>
-      <c r="H82" s="1">
-        <f t="shared" si="18"/>
-        <v>1.6355056417572622E-2</v>
-      </c>
-      <c r="J82" s="3">
         <f t="shared" si="19"/>
         <v>4.9637163926718735</v>
       </c>
+      <c r="H82" s="1">
+        <f t="shared" si="20"/>
+        <v>1.6355056417572622E-2</v>
+      </c>
+      <c r="J82" s="3">
+        <f t="shared" si="21"/>
+        <v>4.9637163926718735</v>
+      </c>
       <c r="K82" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>6.1846659978068277E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M82" s="3">
+        <f t="shared" si="23"/>
+        <v>4.9637163926718735</v>
+      </c>
+      <c r="N82" s="13">
+        <f t="shared" si="24"/>
+        <v>0.64070000000000005</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <f t="shared" si="14"/>
-        <v>5.026548245743669</v>
-      </c>
-      <c r="B83" s="1">
-        <f t="shared" si="15"/>
-        <v>0.65450849718747361</v>
-      </c>
-      <c r="D83" s="3">
         <f t="shared" si="16"/>
         <v>5.026548245743669</v>
       </c>
+      <c r="B83" s="1">
+        <f t="shared" si="17"/>
+        <v>0.65450849718747361</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="18"/>
+        <v>5.026548245743669</v>
+      </c>
       <c r="E83" s="1">
         <v>0.66310000000000002</v>
       </c>
       <c r="G83" s="3">
-        <f t="shared" si="17"/>
-        <v>5.026548245743669</v>
-      </c>
-      <c r="H83" s="1">
-        <f t="shared" si="18"/>
-        <v>8.5915028125264081E-3</v>
-      </c>
-      <c r="J83" s="3">
         <f t="shared" si="19"/>
         <v>5.026548245743669</v>
       </c>
+      <c r="H83" s="1">
+        <f t="shared" si="20"/>
+        <v>8.5915028125264081E-3</v>
+      </c>
+      <c r="J83" s="3">
+        <f t="shared" si="21"/>
+        <v>5.026548245743669</v>
+      </c>
       <c r="K83" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.5491502812526163E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M83" s="3">
+        <f t="shared" si="23"/>
+        <v>5.026548245743669</v>
+      </c>
+      <c r="N83" s="13">
+        <f t="shared" si="24"/>
+        <v>0.66310000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <f t="shared" si="14"/>
-        <v>5.0893800988154645</v>
-      </c>
-      <c r="B84" s="1">
-        <f t="shared" si="15"/>
-        <v>0.68406227634233885</v>
-      </c>
-      <c r="D84" s="3">
         <f t="shared" si="16"/>
         <v>5.0893800988154645</v>
       </c>
+      <c r="B84" s="1">
+        <f t="shared" si="17"/>
+        <v>0.68406227634233885</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="18"/>
+        <v>5.0893800988154645</v>
+      </c>
       <c r="E84" s="1">
         <v>0.68789999999999996</v>
       </c>
       <c r="G84" s="3">
-        <f t="shared" si="17"/>
-        <v>5.0893800988154645</v>
-      </c>
-      <c r="H84" s="1">
-        <f t="shared" si="18"/>
-        <v>3.8377236576611073E-3</v>
-      </c>
-      <c r="J84" s="3">
         <f t="shared" si="19"/>
         <v>5.0893800988154645</v>
       </c>
+      <c r="H84" s="1">
+        <f t="shared" si="20"/>
+        <v>3.8377236576611073E-3</v>
+      </c>
+      <c r="J84" s="3">
+        <f t="shared" si="21"/>
+        <v>5.0893800988154645</v>
+      </c>
       <c r="K84" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.13551568628929384</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M84" s="3">
+        <f t="shared" si="23"/>
+        <v>5.0893800988154645</v>
+      </c>
+      <c r="N84" s="13">
+        <f t="shared" si="24"/>
+        <v>0.68789999999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <f t="shared" si="14"/>
-        <v>5.15221195188726</v>
-      </c>
-      <c r="B85" s="1">
-        <f t="shared" si="15"/>
-        <v>0.712889645782536</v>
-      </c>
-      <c r="D85" s="3">
         <f t="shared" si="16"/>
         <v>5.15221195188726</v>
       </c>
+      <c r="B85" s="1">
+        <f t="shared" si="17"/>
+        <v>0.712889645782536</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="18"/>
+        <v>5.15221195188726</v>
+      </c>
       <c r="E85" s="1">
         <v>0.7137</v>
       </c>
       <c r="G85" s="3">
-        <f t="shared" si="17"/>
-        <v>5.15221195188726</v>
-      </c>
-      <c r="H85" s="1">
-        <f t="shared" si="18"/>
-        <v>8.1035421746400438E-4</v>
-      </c>
-      <c r="J85" s="3">
         <f t="shared" si="19"/>
         <v>5.15221195188726</v>
       </c>
+      <c r="H85" s="1">
+        <f t="shared" si="20"/>
+        <v>8.1035421746400438E-4</v>
+      </c>
+      <c r="J85" s="3">
+        <f t="shared" si="21"/>
+        <v>5.15221195188726</v>
+      </c>
       <c r="K85" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.18128800512565443</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M85" s="3">
+        <f t="shared" si="23"/>
+        <v>5.15221195188726</v>
+      </c>
+      <c r="N85" s="13">
+        <f t="shared" si="24"/>
+        <v>0.7137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <f t="shared" si="14"/>
-        <v>5.2150438049590573</v>
-      </c>
-      <c r="B86" s="1">
-        <f t="shared" si="15"/>
-        <v>0.74087683705085783</v>
-      </c>
-      <c r="D86" s="3">
         <f t="shared" si="16"/>
         <v>5.2150438049590573</v>
       </c>
+      <c r="B86" s="1">
+        <f t="shared" si="17"/>
+        <v>0.74087683705085783</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="18"/>
+        <v>5.2150438049590573</v>
+      </c>
       <c r="E86" s="1">
         <v>0.74419999999999997</v>
       </c>
       <c r="G86" s="3">
-        <f t="shared" si="17"/>
-        <v>5.2150438049590573</v>
-      </c>
-      <c r="H86" s="1">
-        <f t="shared" si="18"/>
-        <v>3.3231629491421444E-3</v>
-      </c>
-      <c r="J86" s="3">
         <f t="shared" si="19"/>
         <v>5.2150438049590573</v>
       </c>
+      <c r="H86" s="1">
+        <f t="shared" si="20"/>
+        <v>3.3231629491421444E-3</v>
+      </c>
+      <c r="J86" s="3">
+        <f t="shared" si="21"/>
+        <v>5.2150438049590573</v>
+      </c>
       <c r="K86" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.23208660251050212</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M86" s="3">
+        <f t="shared" si="23"/>
+        <v>5.2150438049590573</v>
+      </c>
+      <c r="N86" s="13">
+        <f t="shared" si="24"/>
+        <v>0.74419999999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <f t="shared" si="14"/>
-        <v>5.2778756580308528</v>
-      </c>
-      <c r="B87" s="1">
-        <f t="shared" si="15"/>
-        <v>0.76791339748949827</v>
-      </c>
-      <c r="D87" s="3">
         <f t="shared" si="16"/>
         <v>5.2778756580308528</v>
       </c>
+      <c r="B87" s="1">
+        <f t="shared" si="17"/>
+        <v>0.76791339748949827</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="18"/>
+        <v>5.2778756580308528</v>
+      </c>
       <c r="E87" s="1">
         <v>0.76680000000000004</v>
       </c>
       <c r="G87" s="3">
-        <f t="shared" si="17"/>
-        <v>5.2778756580308528</v>
-      </c>
-      <c r="H87" s="1">
-        <f t="shared" si="18"/>
-        <v>1.1133974894982357E-3</v>
-      </c>
-      <c r="J87" s="3">
         <f t="shared" si="19"/>
         <v>5.2778756580308528</v>
       </c>
+      <c r="H87" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1133974894982357E-3</v>
+      </c>
+      <c r="J87" s="3">
+        <f t="shared" si="21"/>
+        <v>5.2778756580308528</v>
+      </c>
       <c r="K87" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.28711035421746384</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M87" s="3">
+        <f t="shared" si="23"/>
+        <v>5.2778756580308528</v>
+      </c>
+      <c r="N87" s="13">
+        <f t="shared" si="24"/>
+        <v>0.76680000000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <f t="shared" si="14"/>
-        <v>5.3407075111026483</v>
-      </c>
-      <c r="B88" s="1">
-        <f t="shared" si="15"/>
-        <v>0.79389262614623646</v>
-      </c>
-      <c r="D88" s="3">
         <f t="shared" si="16"/>
         <v>5.3407075111026483</v>
       </c>
+      <c r="B88" s="1">
+        <f t="shared" si="17"/>
+        <v>0.79389262614623646</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="18"/>
+        <v>5.3407075111026483</v>
+      </c>
       <c r="E88" s="1">
         <v>0.79090000000000005</v>
       </c>
       <c r="G88" s="3">
-        <f t="shared" si="17"/>
-        <v>5.3407075111026483</v>
-      </c>
-      <c r="H88" s="1">
-        <f t="shared" si="18"/>
-        <v>2.9926261462364101E-3</v>
-      </c>
-      <c r="J88" s="3">
         <f t="shared" si="19"/>
         <v>5.3407075111026483</v>
       </c>
+      <c r="H88" s="1">
+        <f t="shared" si="20"/>
+        <v>2.9926261462364101E-3</v>
+      </c>
+      <c r="J88" s="3">
+        <f t="shared" si="21"/>
+        <v>5.3407075111026483</v>
+      </c>
       <c r="K88" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.34549150281252605</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M88" s="3">
+        <f t="shared" si="23"/>
+        <v>5.3407075111026483</v>
+      </c>
+      <c r="N88" s="13">
+        <f t="shared" si="24"/>
+        <v>0.79090000000000005</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <f t="shared" si="14"/>
-        <v>5.4035393641744438</v>
-      </c>
-      <c r="B89" s="1">
-        <f t="shared" si="15"/>
-        <v>0.81871199487434454</v>
-      </c>
-      <c r="D89" s="3">
         <f t="shared" si="16"/>
         <v>5.4035393641744438</v>
       </c>
+      <c r="B89" s="1">
+        <f t="shared" si="17"/>
+        <v>0.81871199487434454</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="18"/>
+        <v>5.4035393641744438</v>
+      </c>
       <c r="E89" s="1">
         <v>0.81920000000000004</v>
       </c>
       <c r="G89" s="3">
-        <f t="shared" si="17"/>
-        <v>5.4035393641744438</v>
-      </c>
-      <c r="H89" s="1">
-        <f t="shared" si="18"/>
-        <v>4.8800512565549958E-4</v>
-      </c>
-      <c r="J89" s="3">
         <f t="shared" si="19"/>
         <v>5.4035393641744438</v>
       </c>
+      <c r="H89" s="1">
+        <f t="shared" si="20"/>
+        <v>4.8800512565549958E-4</v>
+      </c>
+      <c r="J89" s="3">
+        <f t="shared" si="21"/>
+        <v>5.4035393641744438</v>
+      </c>
       <c r="K89" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.40630934270713714</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M89" s="3">
+        <f t="shared" si="23"/>
+        <v>5.4035393641744438</v>
+      </c>
+      <c r="N89" s="13">
+        <f t="shared" si="24"/>
+        <v>0.81920000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <f t="shared" si="14"/>
-        <v>5.4663712172462393</v>
-      </c>
-      <c r="B90" s="1">
-        <f t="shared" si="15"/>
-        <v>0.84227355296434392</v>
-      </c>
-      <c r="D90" s="3">
         <f t="shared" si="16"/>
         <v>5.4663712172462393</v>
       </c>
+      <c r="B90" s="1">
+        <f t="shared" si="17"/>
+        <v>0.84227355296434392</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="18"/>
+        <v>5.4663712172462393</v>
+      </c>
       <c r="E90" s="1">
         <v>0.83840000000000003</v>
       </c>
       <c r="G90" s="3">
-        <f t="shared" si="17"/>
-        <v>5.4663712172462393</v>
-      </c>
-      <c r="H90" s="1">
-        <f t="shared" si="18"/>
-        <v>3.8735529643438849E-3</v>
-      </c>
-      <c r="J90" s="3">
         <f t="shared" si="19"/>
         <v>5.4663712172462393</v>
       </c>
+      <c r="H90" s="1">
+        <f t="shared" si="20"/>
+        <v>3.8735529643438849E-3</v>
+      </c>
+      <c r="J90" s="3">
+        <f t="shared" si="21"/>
+        <v>5.4663712172462393</v>
+      </c>
       <c r="K90" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.46860474023534232</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M90" s="3">
+        <f t="shared" si="23"/>
+        <v>5.4663712172462393</v>
+      </c>
+      <c r="N90" s="13">
+        <f t="shared" si="24"/>
+        <v>0.83840000000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <f t="shared" si="14"/>
-        <v>5.5292030703180357</v>
-      </c>
-      <c r="B91" s="1">
-        <f t="shared" si="15"/>
-        <v>0.86448431371070567</v>
-      </c>
-      <c r="D91" s="3">
         <f t="shared" si="16"/>
         <v>5.5292030703180357</v>
       </c>
+      <c r="B91" s="1">
+        <f t="shared" si="17"/>
+        <v>0.86448431371070567</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="18"/>
+        <v>5.5292030703180357</v>
+      </c>
       <c r="E91" s="1">
         <v>0.85629999999999995</v>
       </c>
       <c r="G91" s="3">
-        <f t="shared" si="17"/>
-        <v>5.5292030703180357</v>
-      </c>
-      <c r="H91" s="1">
-        <f t="shared" si="18"/>
-        <v>8.1843137107057151E-3</v>
-      </c>
-      <c r="J91" s="3">
         <f t="shared" si="19"/>
         <v>5.5292030703180357</v>
       </c>
+      <c r="H91" s="1">
+        <f t="shared" si="20"/>
+        <v>8.1843137107057151E-3</v>
+      </c>
+      <c r="J91" s="3">
+        <f t="shared" si="21"/>
+        <v>5.5292030703180357</v>
+      </c>
       <c r="K91" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.53139525976465629</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M91" s="3">
+        <f t="shared" si="23"/>
+        <v>5.5292030703180357</v>
+      </c>
+      <c r="N91" s="13">
+        <f t="shared" si="24"/>
+        <v>0.85629999999999995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <f t="shared" si="14"/>
-        <v>5.5920349233898321</v>
-      </c>
-      <c r="B92" s="1">
-        <f t="shared" si="15"/>
-        <v>0.88525662138789463</v>
-      </c>
-      <c r="D92" s="3">
         <f t="shared" si="16"/>
         <v>5.5920349233898321</v>
       </c>
+      <c r="B92" s="1">
+        <f t="shared" si="17"/>
+        <v>0.88525662138789463</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="18"/>
+        <v>5.5920349233898321</v>
+      </c>
       <c r="E92" s="1">
         <v>0.87875000000000003</v>
       </c>
       <c r="G92" s="3">
-        <f t="shared" si="17"/>
-        <v>5.5920349233898321</v>
-      </c>
-      <c r="H92" s="1">
-        <f t="shared" si="18"/>
-        <v>6.5066213878945955E-3</v>
-      </c>
-      <c r="J92" s="3">
         <f t="shared" si="19"/>
         <v>5.5920349233898321</v>
       </c>
+      <c r="H92" s="1">
+        <f t="shared" si="20"/>
+        <v>6.5066213878945955E-3</v>
+      </c>
+      <c r="J92" s="3">
+        <f t="shared" si="21"/>
+        <v>5.5920349233898321</v>
+      </c>
       <c r="K92" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.59369065729286252</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M92" s="3">
+        <f t="shared" si="23"/>
+        <v>5.5920349233898321</v>
+      </c>
+      <c r="N92" s="13">
+        <f t="shared" si="24"/>
+        <v>0.87880000000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <f t="shared" si="14"/>
-        <v>5.6548667764616276</v>
-      </c>
-      <c r="B93" s="1">
-        <f t="shared" si="15"/>
-        <v>0.90450849718747361</v>
-      </c>
-      <c r="D93" s="3">
         <f t="shared" si="16"/>
         <v>5.6548667764616276</v>
       </c>
+      <c r="B93" s="1">
+        <f t="shared" si="17"/>
+        <v>0.90450849718747361</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="18"/>
+        <v>5.6548667764616276</v>
+      </c>
       <c r="E93" s="1">
         <v>0.90075000000000005</v>
       </c>
       <c r="G93" s="3">
-        <f t="shared" si="17"/>
-        <v>5.6548667764616276</v>
-      </c>
-      <c r="H93" s="1">
-        <f t="shared" si="18"/>
-        <v>3.758497187473564E-3</v>
-      </c>
-      <c r="J93" s="3">
         <f t="shared" si="19"/>
         <v>5.6548667764616276</v>
       </c>
+      <c r="H93" s="1">
+        <f t="shared" si="20"/>
+        <v>3.758497187473564E-3</v>
+      </c>
+      <c r="J93" s="3">
+        <f t="shared" si="21"/>
+        <v>5.6548667764616276</v>
+      </c>
       <c r="K93" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.65450849718747361</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M93" s="3">
+        <f t="shared" si="23"/>
+        <v>5.6548667764616276</v>
+      </c>
+      <c r="N93" s="13">
+        <f t="shared" si="24"/>
+        <v>0.90080000000000005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <f t="shared" si="14"/>
-        <v>5.7176986295334231</v>
-      </c>
-      <c r="B94" s="1">
-        <f t="shared" si="15"/>
-        <v>0.92216396275100732</v>
-      </c>
-      <c r="D94" s="3">
         <f t="shared" si="16"/>
         <v>5.7176986295334231</v>
       </c>
+      <c r="B94" s="1">
+        <f t="shared" si="17"/>
+        <v>0.92216396275100732</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="18"/>
+        <v>5.7176986295334231</v>
+      </c>
       <c r="E94" s="1">
         <v>0.91039999999999999</v>
       </c>
       <c r="G94" s="3">
-        <f t="shared" si="17"/>
-        <v>5.7176986295334231</v>
-      </c>
-      <c r="H94" s="1">
-        <f t="shared" si="18"/>
-        <v>1.1763962751007329E-2</v>
-      </c>
-      <c r="J94" s="3">
         <f t="shared" si="19"/>
         <v>5.7176986295334231</v>
       </c>
+      <c r="H94" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1763962751007329E-2</v>
+      </c>
+      <c r="J94" s="3">
+        <f t="shared" si="21"/>
+        <v>5.7176986295334231</v>
+      </c>
       <c r="K94" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.71288964578253577</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M94" s="3">
+        <f t="shared" si="23"/>
+        <v>5.7176986295334231</v>
+      </c>
+      <c r="N94" s="13">
+        <f t="shared" si="24"/>
+        <v>0.91039999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <f t="shared" si="14"/>
-        <v>5.7805304826052186</v>
-      </c>
-      <c r="B95" s="1">
-        <f t="shared" si="15"/>
-        <v>0.93815334002193151</v>
-      </c>
-      <c r="D95" s="3">
         <f t="shared" si="16"/>
         <v>5.7805304826052186</v>
       </c>
+      <c r="B95" s="1">
+        <f t="shared" si="17"/>
+        <v>0.93815334002193151</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="18"/>
+        <v>5.7805304826052186</v>
+      </c>
       <c r="E95" s="1">
         <v>0.92889999999999995</v>
       </c>
       <c r="G95" s="3">
-        <f t="shared" si="17"/>
-        <v>5.7805304826052186</v>
-      </c>
-      <c r="H95" s="1">
-        <f t="shared" si="18"/>
-        <v>9.2533400219315665E-3</v>
-      </c>
-      <c r="J95" s="3">
         <f t="shared" si="19"/>
         <v>5.7805304826052186</v>
       </c>
+      <c r="H95" s="1">
+        <f t="shared" si="20"/>
+        <v>9.2533400219315665E-3</v>
+      </c>
+      <c r="J95" s="3">
+        <f t="shared" si="21"/>
+        <v>5.7805304826052186</v>
+      </c>
       <c r="K95" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.7679133974894975</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M95" s="3">
+        <f t="shared" si="23"/>
+        <v>5.7805304826052186</v>
+      </c>
+      <c r="N95" s="13">
+        <f t="shared" si="24"/>
+        <v>0.92889999999999995</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <f t="shared" si="14"/>
-        <v>5.843362335677015</v>
-      </c>
-      <c r="B96" s="1">
-        <f t="shared" si="15"/>
-        <v>0.95241352623300957</v>
-      </c>
-      <c r="D96" s="3">
         <f t="shared" si="16"/>
         <v>5.843362335677015</v>
       </c>
+      <c r="B96" s="1">
+        <f t="shared" si="17"/>
+        <v>0.95241352623300957</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="18"/>
+        <v>5.843362335677015</v>
+      </c>
       <c r="E96" s="1">
         <v>0.94259999999999999</v>
       </c>
       <c r="G96" s="3">
-        <f t="shared" si="17"/>
-        <v>5.843362335677015</v>
-      </c>
-      <c r="H96" s="1">
-        <f t="shared" si="18"/>
-        <v>9.8135262330095729E-3</v>
-      </c>
-      <c r="J96" s="3">
         <f t="shared" si="19"/>
         <v>5.843362335677015</v>
       </c>
+      <c r="H96" s="1">
+        <f t="shared" si="20"/>
+        <v>9.8135262330095729E-3</v>
+      </c>
+      <c r="J96" s="3">
+        <f t="shared" si="21"/>
+        <v>5.843362335677015</v>
+      </c>
       <c r="K96" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.81871199487434454</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M96" s="3">
+        <f t="shared" si="23"/>
+        <v>5.843362335677015</v>
+      </c>
+      <c r="N96" s="13">
+        <f t="shared" si="24"/>
+        <v>0.94259999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <f t="shared" si="14"/>
-        <v>5.9061941887488114</v>
-      </c>
-      <c r="B97" s="1">
-        <f t="shared" si="15"/>
-        <v>0.96488824294412578</v>
-      </c>
-      <c r="D97" s="3">
         <f t="shared" si="16"/>
         <v>5.9061941887488114</v>
       </c>
+      <c r="B97" s="1">
+        <f t="shared" si="17"/>
+        <v>0.96488824294412578</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="18"/>
+        <v>5.9061941887488114</v>
+      </c>
       <c r="E97" s="1">
         <v>0.95355000000000001</v>
       </c>
       <c r="G97" s="3">
-        <f t="shared" si="17"/>
-        <v>5.9061941887488114</v>
-      </c>
-      <c r="H97" s="1">
-        <f t="shared" si="18"/>
-        <v>1.1338242944125776E-2</v>
-      </c>
-      <c r="J97" s="3">
         <f t="shared" si="19"/>
         <v>5.9061941887488114</v>
       </c>
+      <c r="H97" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1338242944125776E-2</v>
+      </c>
+      <c r="J97" s="3">
+        <f t="shared" si="21"/>
+        <v>5.9061941887488114</v>
+      </c>
       <c r="K97" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.86448431371070589</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M97" s="3">
+        <f t="shared" si="23"/>
+        <v>5.9061941887488114</v>
+      </c>
+      <c r="N97" s="13">
+        <f t="shared" si="24"/>
+        <v>0.9536</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <f t="shared" si="14"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="B98" s="1">
-        <f t="shared" si="15"/>
-        <v>0.9755282581475766</v>
-      </c>
-      <c r="D98" s="3">
         <f t="shared" si="16"/>
         <v>5.9690260418206069</v>
       </c>
+      <c r="B98" s="1">
+        <f t="shared" si="17"/>
+        <v>0.9755282581475766</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="18"/>
+        <v>5.9690260418206069</v>
+      </c>
       <c r="E98" s="1">
         <v>0.96309999999999996</v>
       </c>
       <c r="G98" s="3">
-        <f t="shared" si="17"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="H98" s="1">
-        <f t="shared" si="18"/>
-        <v>1.2428258147576643E-2</v>
-      </c>
-      <c r="J98" s="3">
         <f t="shared" si="19"/>
         <v>5.9690260418206069</v>
       </c>
+      <c r="H98" s="1">
+        <f t="shared" si="20"/>
+        <v>1.2428258147576643E-2</v>
+      </c>
+      <c r="J98" s="3">
+        <f t="shared" si="21"/>
+        <v>5.9690260418206069</v>
+      </c>
       <c r="K98" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.90450849718747361</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M98" s="3">
+        <f t="shared" si="23"/>
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="N98" s="13">
+        <f t="shared" si="24"/>
+        <v>0.96309999999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <f t="shared" si="14"/>
-        <v>6.0318578948924024</v>
-      </c>
-      <c r="B99" s="1">
-        <f t="shared" ref="B99:B103" si="21">ABS(COS(A99/2))^2</f>
-        <v>0.98429158056431543</v>
-      </c>
-      <c r="D99" s="3">
         <f t="shared" si="16"/>
         <v>6.0318578948924024</v>
       </c>
+      <c r="B99" s="1">
+        <f t="shared" ref="B99:B103" si="25">ABS(COS(A99/2))^2</f>
+        <v>0.98429158056431543</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="18"/>
+        <v>6.0318578948924024</v>
+      </c>
       <c r="E99" s="1">
         <v>0.97319999999999995</v>
       </c>
       <c r="G99" s="3">
-        <f t="shared" si="17"/>
-        <v>6.0318578948924024</v>
-      </c>
-      <c r="H99" s="1">
-        <f t="shared" si="18"/>
-        <v>1.1091580564315473E-2</v>
-      </c>
-      <c r="J99" s="3">
         <f t="shared" si="19"/>
         <v>6.0318578948924024</v>
       </c>
+      <c r="H99" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1091580564315473E-2</v>
+      </c>
+      <c r="J99" s="3">
+        <f t="shared" si="21"/>
+        <v>6.0318578948924024</v>
+      </c>
       <c r="K99" s="1">
-        <f t="shared" ref="K99:K103" si="22">ABS(COS(J99))^2</f>
+        <f t="shared" ref="K99:K103" si="26">ABS(COS(J99))^2</f>
         <v>0.93815334002193151</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M99" s="3">
+        <f t="shared" si="23"/>
+        <v>6.0318578948924024</v>
+      </c>
+      <c r="N99" s="13">
+        <f t="shared" si="24"/>
+        <v>0.97319999999999995</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <f t="shared" si="14"/>
-        <v>6.0946897479641988</v>
-      </c>
-      <c r="B100" s="1">
-        <f t="shared" si="21"/>
-        <v>0.99114362536434431</v>
-      </c>
-      <c r="D100" s="3">
         <f t="shared" si="16"/>
         <v>6.0946897479641988</v>
       </c>
+      <c r="B100" s="1">
+        <f t="shared" si="25"/>
+        <v>0.99114362536434431</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="18"/>
+        <v>6.0946897479641988</v>
+      </c>
       <c r="E100" s="1">
         <v>0.98035000000000005</v>
       </c>
       <c r="G100" s="3">
-        <f t="shared" si="17"/>
-        <v>6.0946897479641988</v>
-      </c>
-      <c r="H100" s="1">
-        <f t="shared" si="18"/>
-        <v>1.079362536434425E-2</v>
-      </c>
-      <c r="J100" s="3">
         <f t="shared" si="19"/>
         <v>6.0946897479641988</v>
       </c>
+      <c r="H100" s="1">
+        <f t="shared" si="20"/>
+        <v>1.079362536434425E-2</v>
+      </c>
+      <c r="J100" s="3">
+        <f t="shared" si="21"/>
+        <v>6.0946897479641988</v>
+      </c>
       <c r="K100" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.96488824294412578</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M100" s="3">
+        <f t="shared" si="23"/>
+        <v>6.0946897479641988</v>
+      </c>
+      <c r="N100" s="13">
+        <f t="shared" si="24"/>
+        <v>0.98040000000000005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <f t="shared" si="14"/>
-        <v>6.1575216010359943</v>
-      </c>
-      <c r="B101" s="1">
-        <f t="shared" si="21"/>
-        <v>0.99605735065723888</v>
-      </c>
-      <c r="D101" s="3">
         <f t="shared" si="16"/>
         <v>6.1575216010359943</v>
       </c>
+      <c r="B101" s="1">
+        <f t="shared" si="25"/>
+        <v>0.99605735065723888</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="18"/>
+        <v>6.1575216010359943</v>
+      </c>
       <c r="E101" s="1">
         <v>0.98445000000000005</v>
       </c>
       <c r="G101" s="3">
-        <f t="shared" si="17"/>
-        <v>6.1575216010359943</v>
-      </c>
-      <c r="H101" s="1">
-        <f t="shared" si="18"/>
-        <v>1.1607350657238835E-2</v>
-      </c>
-      <c r="J101" s="3">
         <f t="shared" si="19"/>
         <v>6.1575216010359943</v>
       </c>
+      <c r="H101" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1607350657238835E-2</v>
+      </c>
+      <c r="J101" s="3">
+        <f t="shared" si="21"/>
+        <v>6.1575216010359943</v>
+      </c>
       <c r="K101" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.98429158056431543</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M101" s="3">
+        <f t="shared" si="23"/>
+        <v>6.1575216010359943</v>
+      </c>
+      <c r="N101" s="13">
+        <f t="shared" si="24"/>
+        <v>0.98440000000000005</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <f t="shared" si="14"/>
-        <v>6.2203534541077907</v>
-      </c>
-      <c r="B102" s="1">
-        <f t="shared" si="21"/>
-        <v>0.99901336421413589</v>
-      </c>
-      <c r="D102" s="3">
         <f t="shared" si="16"/>
         <v>6.2203534541077907</v>
       </c>
+      <c r="B102" s="1">
+        <f t="shared" si="25"/>
+        <v>0.99901336421413589</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="18"/>
+        <v>6.2203534541077907</v>
+      </c>
       <c r="E102" s="1">
         <v>0.98904999999999998</v>
       </c>
       <c r="G102" s="3">
-        <f t="shared" si="17"/>
-        <v>6.2203534541077907</v>
-      </c>
-      <c r="H102" s="1">
-        <f t="shared" si="18"/>
-        <v>9.9633642141359058E-3</v>
-      </c>
-      <c r="J102" s="3">
         <f t="shared" si="19"/>
         <v>6.2203534541077907</v>
       </c>
+      <c r="H102" s="1">
+        <f t="shared" si="20"/>
+        <v>9.9633642141359058E-3</v>
+      </c>
+      <c r="J102" s="3">
+        <f t="shared" si="21"/>
+        <v>6.2203534541077907</v>
+      </c>
       <c r="K102" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.99605735065723888</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M102" s="3">
+        <f t="shared" si="23"/>
+        <v>6.2203534541077907</v>
+      </c>
+      <c r="N102" s="13">
+        <f t="shared" si="24"/>
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
-        <f t="shared" si="14"/>
-        <v>6.2831853071795862</v>
-      </c>
-      <c r="B103" s="5">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-      <c r="D103" s="4">
         <f t="shared" si="16"/>
         <v>6.2831853071795862</v>
       </c>
-      <c r="E103" s="1">
+      <c r="B103" s="5">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="D103" s="4">
+        <f t="shared" si="18"/>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="E103" s="5">
         <v>0.98785000000000001</v>
       </c>
       <c r="G103" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>6.2831853071795862</v>
       </c>
       <c r="H103" s="5">
@@ -3913,22 +4729,31 @@
         <v>1.2149999999999994E-2</v>
       </c>
       <c r="J103" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.2831853071795862</v>
       </c>
       <c r="K103" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
+      <c r="M103" s="4">
+        <f t="shared" si="23"/>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="N103" s="14">
+        <f t="shared" si="24"/>
+        <v>0.98780000000000001</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>